<commit_message>
doc for html and nlp as well as modifications for testing.py
</commit_message>
<xml_diff>
--- a/test_data/DataSetWithFullResults.xlsx
+++ b/test_data/DataSetWithFullResults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobfehn/Documents/Uni/7. Semester/Thesis/Webservice/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737151F7-9B71-5F47-A86B-E88D3EE3D995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0743317-6EF9-C948-AC0B-8C43E8B3FC4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" xr2:uid="{9DEADDE0-F9AA-D64D-B8E2-B7DD8B179BBE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{9DEADDE0-F9AA-D64D-B8E2-B7DD8B179BBE}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3077" uniqueCount="1479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3079" uniqueCount="1477">
   <si>
     <t>Date First</t>
   </si>
@@ -3686,9 +3686,6 @@
     <t>C: 0 ; M: 28 + 2 ;</t>
   </si>
   <si>
-    <t>C: 0 ; M: 6 + 5 (6) + 5 (5) ;</t>
-  </si>
-  <si>
     <t>C: 0 ; M: 1 ;</t>
   </si>
   <si>
@@ -3734,9 +3731,6 @@
     <t>C: 0 ; M: 2 + 2 + 7 + 10 ;</t>
   </si>
   <si>
-    <t>C: 0 ; M: 0 ; OVERFLOW</t>
-  </si>
-  <si>
     <t>https://eur-lex.europa.eu/legal-content/EN/TXT/HTML/?uri=CELEX:02010D0712-20111221</t>
   </si>
   <si>
@@ -4010,15 +4004,6 @@
     <t>C: 0 ; M: 6 ;</t>
   </si>
   <si>
-    <t xml:space="preserve">C: 0 ; M: 1 (A: -3) ; </t>
-  </si>
-  <si>
-    <t>C: 0 ; M: 68  + 38 + 65 + 19 + 1 + 15 + 1 + 5 ;</t>
-  </si>
-  <si>
-    <t>C: 0 ; M: (-9) + 38 + 65 + 19 + 1 + 15 + 1 + 5 ;</t>
-  </si>
-  <si>
     <t>TEST THIS</t>
   </si>
   <si>
@@ -4034,15 +4019,6 @@
     <t>C: 0 ; M: 1 + 3 + 3 + 2 + 1 + 2 + 7 + 3 ;</t>
   </si>
   <si>
-    <t>C: 0 ; M: (-1) + 26 + 3 + 182 + 10 ;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C: 1 ; M: 15 + 9 + 1 + 1 + 2 + 21 + 3 + 3 + 1 + 17 + 1 + 5 + 4 + 2 + 11 + 4 + 7 + 18 + 1 + 4; </t>
-  </si>
-  <si>
-    <t>C: 0 ; M: (-1) + 1 ;</t>
-  </si>
-  <si>
     <t>C: 2 ; M: 1 + 3 + 1 + 2 + 3 + 6 + 1 + 4 ;</t>
   </si>
   <si>
@@ -4055,24 +4031,15 @@
     <t>C: 0 ; M: 7 + 10 ;</t>
   </si>
   <si>
-    <t>C: 0 ; M: (-3) + 7 + 6 + 2 + 5 ;</t>
-  </si>
-  <si>
     <t>C: 0 ; M: 2 + 9 + 1 + 33 + 1 + 10 ;</t>
   </si>
   <si>
-    <t>C: 0 ; M: (-3) + 4 ;</t>
-  </si>
-  <si>
     <t>C: 0 ; M: 3 + 3 + 3 + 5 + 7 ;</t>
   </si>
   <si>
     <t>C: 0 ; M: 12 + 3 ;</t>
   </si>
   <si>
-    <t>C: 0 ; M(A) 2 ;</t>
-  </si>
-  <si>
     <t>C: 0 ; M: 34 ;</t>
   </si>
   <si>
@@ -4457,15 +4424,9 @@
     <t>C: 2 ; M: 1 ;</t>
   </si>
   <si>
-    <t>Title Mod.</t>
-  </si>
-  <si>
     <t>C: 0 ; M: 2 + 5 + 26 + 3 + 182 + 10 ;</t>
   </si>
   <si>
-    <t>C: 75 ; M: 3 + 1 + 5 + 5 + 16 + 1 + 1 + 6 + 2 + 1 + 1 + 1 + 2 + 2 + 8 + 1 + 2 + 9 + 1 + 33 + 1 + 10 ;</t>
-  </si>
-  <si>
     <t>C: 1 ; M: 11 + 1 + 4 ;</t>
   </si>
   <si>
@@ -4487,13 +4448,46 @@
     <t>C: 15 + 6 ; M: 5 ;</t>
   </si>
   <si>
-    <t>Not</t>
-  </si>
-  <si>
     <t>C: 4 ; M: 1 ;</t>
   </si>
   <si>
-    <t>Test for Newest</t>
+    <t>old, unmarked deletion</t>
+  </si>
+  <si>
+    <t>edge case for mods in title and introduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C: 0 ; M: 1 ; </t>
+  </si>
+  <si>
+    <t>C: 0 ; M: 26 + 3 + 182 + 10 ;</t>
+  </si>
+  <si>
+    <t>C: 0 ; M: 7 + 6 + 2 + 5 ;</t>
+  </si>
+  <si>
+    <t>A instead for M</t>
+  </si>
+  <si>
+    <t>C: 0 ; M: 6 + 5 + 5 ;</t>
+  </si>
+  <si>
+    <t>C: 0 ; M: 38 + 65 + 19 + 1 + 15 + 1 + 5 ;</t>
+  </si>
+  <si>
+    <t>C: 0 ; M: 68 + 38 + 65 + 19 + 1 + 15 + 1 + 5 ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C: 1 ; M: 15 + 9 + 1 + 1 + 2 + 21 + 3 + 3 + 1 + 17 + 1 + 5 + 4 + 2 + 11 + 4 + 7 + 18 + 1 + 4 ; </t>
+  </si>
+  <si>
+    <t>C: 75 ; M: 3 + 1 + 5 + 5 + 16 + 1 + 1 + 5 + 2 + 1 + 1 + 1 + 1 + 2 + 2 + 8 + 1 + 2 + 9 + 1 + 33 + 1 + 10 ;</t>
+  </si>
+  <si>
+    <t>M17 with 0 mods (M16: 4-&gt;3)</t>
+  </si>
+  <si>
+    <t>M13 with 0 mods (M9: 6-&gt;5)</t>
   </si>
 </sst>
 </file>
@@ -4930,8 +4924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89784638-68A1-8249-8E72-BC8438B6227E}">
   <dimension ref="B1:T277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O59" sqref="O59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4957,12 +4951,12 @@
     <col min="19" max="19" width="29.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:19" x14ac:dyDescent="0.2">
       <c r="L1" t="s">
         <v>758</v>
       </c>
     </row>
-    <row r="2" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -5012,13 +5006,13 @@
         <v>1205</v>
       </c>
       <c r="R2" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
       <c r="S2" t="s">
-        <v>1391</v>
-      </c>
-    </row>
-    <row r="3" spans="2:20" ht="18" x14ac:dyDescent="0.2">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="3" spans="2:19" ht="18" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
@@ -5062,16 +5056,16 @@
         <v>44978</v>
       </c>
       <c r="Q3" t="s">
-        <v>1476</v>
+        <v>430</v>
       </c>
       <c r="R3" t="s">
-        <v>1476</v>
+        <v>430</v>
       </c>
       <c r="S3" t="s">
-        <v>1476</v>
-      </c>
-    </row>
-    <row r="4" spans="2:20" ht="18" x14ac:dyDescent="0.2">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" ht="18" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -5121,7 +5115,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="5" spans="2:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:19" ht="18" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
@@ -5165,16 +5159,16 @@
         <v>44978</v>
       </c>
       <c r="Q5" t="s">
-        <v>1476</v>
+        <v>430</v>
       </c>
       <c r="R5" t="s">
-        <v>1476</v>
+        <v>430</v>
       </c>
       <c r="S5" t="s">
-        <v>1476</v>
-      </c>
-    </row>
-    <row r="6" spans="2:20" ht="18" x14ac:dyDescent="0.2">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" ht="18" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -5200,7 +5194,7 @@
         <v>2021</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>1311</v>
+        <v>1309</v>
       </c>
       <c r="K6">
         <v>3</v>
@@ -5221,16 +5215,16 @@
         <v>44978</v>
       </c>
       <c r="Q6" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
       <c r="R6" t="s">
-        <v>1312</v>
+        <v>1310</v>
       </c>
       <c r="S6" t="s">
-        <v>1275</v>
-      </c>
-    </row>
-    <row r="7" spans="2:20" ht="18" x14ac:dyDescent="0.2">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" ht="18" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
@@ -5274,16 +5268,16 @@
         <v>44978</v>
       </c>
       <c r="Q7" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="R7" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="S7" t="s">
-        <v>1390</v>
-      </c>
-    </row>
-    <row r="8" spans="2:20" ht="18" x14ac:dyDescent="0.2">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" ht="18" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
@@ -5330,13 +5324,13 @@
         <v>1208</v>
       </c>
       <c r="R8" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="S8" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="9" spans="2:20" ht="18" x14ac:dyDescent="0.2">
+        <v>1381</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" ht="18" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
@@ -5377,7 +5371,7 @@
         <v>44978</v>
       </c>
       <c r="Q9" t="s">
-        <v>1457</v>
+        <v>1446</v>
       </c>
       <c r="R9" t="s">
         <v>430</v>
@@ -5386,7 +5380,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="10" spans="2:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:19" ht="18" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
@@ -5430,16 +5424,16 @@
         <v>44978</v>
       </c>
       <c r="Q10" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="R10" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="S10" t="s">
-        <v>1210</v>
-      </c>
-    </row>
-    <row r="11" spans="2:20" ht="18" x14ac:dyDescent="0.2">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" ht="18" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
@@ -5486,19 +5480,16 @@
         <v>44978</v>
       </c>
       <c r="Q11" t="s">
-        <v>1394</v>
+        <v>1383</v>
       </c>
       <c r="R11" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="S11" t="s">
-        <v>1275</v>
-      </c>
-      <c r="T11" t="s">
-        <v>1478</v>
-      </c>
-    </row>
-    <row r="12" spans="2:20" ht="18" x14ac:dyDescent="0.2">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" ht="18" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
@@ -5542,16 +5533,16 @@
         <v>44978</v>
       </c>
       <c r="Q12" t="s">
-        <v>1209</v>
+        <v>1470</v>
       </c>
       <c r="R12" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="S12" t="s">
-        <v>1393</v>
-      </c>
-    </row>
-    <row r="13" spans="2:20" ht="18" x14ac:dyDescent="0.2">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" ht="18" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
@@ -5592,7 +5583,7 @@
         <v>44978</v>
       </c>
       <c r="Q13" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R13" t="s">
         <v>430</v>
@@ -5601,7 +5592,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="14" spans="2:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:19" ht="18" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
@@ -5645,16 +5636,16 @@
         <v>44978</v>
       </c>
       <c r="Q14" t="s">
+        <v>1209</v>
+      </c>
+      <c r="R14" t="s">
+        <v>1209</v>
+      </c>
+      <c r="S14" t="s">
         <v>1210</v>
       </c>
-      <c r="R14" t="s">
-        <v>1210</v>
-      </c>
-      <c r="S14" t="s">
-        <v>1211</v>
-      </c>
-    </row>
-    <row r="15" spans="2:20" ht="18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="2:19" ht="18" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>15</v>
       </c>
@@ -5695,7 +5686,7 @@
         <v>44978</v>
       </c>
       <c r="Q15" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="R15" t="s">
         <v>430</v>
@@ -5704,7 +5695,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="16" spans="2:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:19" ht="18" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>16</v>
       </c>
@@ -5745,7 +5736,7 @@
         <v>44978</v>
       </c>
       <c r="Q16" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R16" t="s">
         <v>430</v>
@@ -5794,20 +5785,20 @@
       <c r="N17" t="s">
         <v>800</v>
       </c>
+      <c r="O17" t="s">
+        <v>1465</v>
+      </c>
       <c r="P17" s="4">
         <v>44978</v>
       </c>
       <c r="Q17" t="s">
-        <v>1465</v>
+        <v>1454</v>
       </c>
       <c r="R17" t="s">
-        <v>1465</v>
+        <v>1454</v>
       </c>
       <c r="S17" t="s">
-        <v>1210</v>
-      </c>
-      <c r="T17" t="s">
-        <v>1466</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="18" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -5854,13 +5845,13 @@
         <v>44978</v>
       </c>
       <c r="Q18" t="s">
-        <v>1395</v>
+        <v>1384</v>
       </c>
       <c r="R18" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="S18" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="19" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -5904,7 +5895,7 @@
         <v>44978</v>
       </c>
       <c r="Q19" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R19" t="s">
         <v>430</v>
@@ -5954,7 +5945,7 @@
         <v>44978</v>
       </c>
       <c r="Q20" t="s">
-        <v>1400</v>
+        <v>1389</v>
       </c>
       <c r="R20" t="s">
         <v>430</v>
@@ -6007,13 +5998,13 @@
         <v>44978</v>
       </c>
       <c r="Q21" t="s">
-        <v>1359</v>
+        <v>1348</v>
       </c>
       <c r="R21" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="S21" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="22" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -6063,13 +6054,13 @@
         <v>44978</v>
       </c>
       <c r="Q22" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="R22" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="S22" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="23" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -6119,16 +6110,16 @@
         <v>44978</v>
       </c>
       <c r="Q23" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R23" t="s">
-        <v>1317</v>
+        <v>1466</v>
       </c>
       <c r="S23" t="s">
-        <v>1396</v>
+        <v>1385</v>
       </c>
       <c r="T23" t="s">
-        <v>1320</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="24" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -6172,7 +6163,7 @@
         <v>44991</v>
       </c>
       <c r="Q24" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="R24" t="s">
         <v>430</v>
@@ -6225,13 +6216,13 @@
         <v>44991</v>
       </c>
       <c r="Q25" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="R25" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="S25" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="26" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -6278,13 +6269,13 @@
         <v>44991</v>
       </c>
       <c r="Q26" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="R26" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="S26" t="s">
-        <v>1397</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="27" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -6328,7 +6319,7 @@
         <v>44991</v>
       </c>
       <c r="Q27" t="s">
-        <v>1400</v>
+        <v>1389</v>
       </c>
       <c r="R27" t="s">
         <v>430</v>
@@ -6378,7 +6369,7 @@
         <v>44991</v>
       </c>
       <c r="Q28" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R28" t="s">
         <v>430</v>
@@ -6428,7 +6419,7 @@
         <v>44991</v>
       </c>
       <c r="Q29" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R29" t="s">
         <v>430</v>
@@ -6481,13 +6472,13 @@
         <v>44991</v>
       </c>
       <c r="Q30" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R30" t="s">
+        <v>1214</v>
+      </c>
+      <c r="S30" t="s">
         <v>1215</v>
-      </c>
-      <c r="R30" t="s">
-        <v>1215</v>
-      </c>
-      <c r="S30" t="s">
-        <v>1216</v>
       </c>
     </row>
     <row r="31" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -6534,13 +6525,13 @@
         <v>44991</v>
       </c>
       <c r="Q31" t="s">
-        <v>1398</v>
+        <v>1387</v>
       </c>
       <c r="R31" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
       <c r="S31" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="32" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -6584,7 +6575,7 @@
         <v>44991</v>
       </c>
       <c r="Q32" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R32" t="s">
         <v>430</v>
@@ -6634,7 +6625,7 @@
         <v>44991</v>
       </c>
       <c r="Q33" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="R33" t="s">
         <v>430</v>
@@ -6687,13 +6678,13 @@
         <v>44991</v>
       </c>
       <c r="Q34" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
       <c r="R34" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
       <c r="S34" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="35" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -6740,16 +6731,16 @@
         <v>44991</v>
       </c>
       <c r="Q35" t="s">
-        <v>1318</v>
+        <v>1472</v>
       </c>
       <c r="R35" t="s">
-        <v>1319</v>
+        <v>1471</v>
       </c>
       <c r="S35" t="s">
-        <v>1399</v>
+        <v>1388</v>
       </c>
       <c r="T35" t="s">
-        <v>1320</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="36" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -6793,13 +6784,13 @@
         <v>44992</v>
       </c>
       <c r="Q36" t="s">
-        <v>1283</v>
+        <v>1281</v>
       </c>
       <c r="R36" t="s">
-        <v>449</v>
+        <v>430</v>
       </c>
       <c r="S36" t="s">
-        <v>449</v>
+        <v>430</v>
       </c>
     </row>
     <row r="37" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -6843,7 +6834,7 @@
         <v>44992</v>
       </c>
       <c r="Q37" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="R37" t="s">
         <v>430</v>
@@ -6896,13 +6887,13 @@
         <v>44992</v>
       </c>
       <c r="Q38" t="s">
-        <v>1380</v>
+        <v>1369</v>
       </c>
       <c r="R38" t="s">
-        <v>1381</v>
+        <v>1370</v>
       </c>
       <c r="S38" t="s">
-        <v>1400</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="39" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -6949,13 +6940,13 @@
         <v>44992</v>
       </c>
       <c r="Q39" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="R39" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="S39" t="s">
-        <v>1401</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="40" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -7002,13 +6993,13 @@
         <v>44992</v>
       </c>
       <c r="Q40" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="R40" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="S40" t="s">
-        <v>1402</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="41" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -7055,13 +7046,13 @@
         <v>44992</v>
       </c>
       <c r="Q41" t="s">
-        <v>1403</v>
+        <v>1392</v>
       </c>
       <c r="R41" t="s">
-        <v>1322</v>
+        <v>1317</v>
       </c>
       <c r="S41" t="s">
-        <v>1404</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="42" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -7108,13 +7099,13 @@
         <v>44992</v>
       </c>
       <c r="Q42" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="R42" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="S42" t="s">
-        <v>1405</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="43" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -7161,13 +7152,13 @@
         <v>44992</v>
       </c>
       <c r="Q43" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="R43" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="S43" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="44" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -7214,13 +7205,13 @@
         <v>44992</v>
       </c>
       <c r="Q44" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="R44" t="s">
-        <v>1323</v>
+        <v>1318</v>
       </c>
       <c r="S44" t="s">
-        <v>1363</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="45" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -7264,7 +7255,7 @@
         <v>44992</v>
       </c>
       <c r="Q45" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R45" t="s">
         <v>430</v>
@@ -7317,13 +7308,13 @@
         <v>44992</v>
       </c>
       <c r="Q46" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="R46" t="s">
-        <v>1324</v>
+        <v>1319</v>
       </c>
       <c r="S46" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="47" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -7370,13 +7361,13 @@
         <v>44992</v>
       </c>
       <c r="Q47" t="s">
+        <v>1455</v>
+      </c>
+      <c r="R47" t="s">
         <v>1467</v>
       </c>
-      <c r="R47" t="s">
-        <v>1325</v>
-      </c>
       <c r="S47" t="s">
-        <v>1395</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="48" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -7423,13 +7414,13 @@
         <v>44992</v>
       </c>
       <c r="Q48" t="s">
-        <v>1406</v>
+        <v>1395</v>
       </c>
       <c r="R48" t="s">
-        <v>1326</v>
+        <v>1473</v>
       </c>
       <c r="S48" t="s">
-        <v>1407</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="49" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -7476,13 +7467,13 @@
         <v>44992</v>
       </c>
       <c r="Q49" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R49" t="s">
-        <v>1327</v>
+        <v>1209</v>
       </c>
       <c r="S49" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="50" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -7529,13 +7520,13 @@
         <v>44992</v>
       </c>
       <c r="Q50" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="R50" t="s">
-        <v>1328</v>
+        <v>1320</v>
       </c>
       <c r="S50" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="51" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -7582,16 +7573,16 @@
         <v>44992</v>
       </c>
       <c r="Q51" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="R51" t="s">
-        <v>1329</v>
+        <v>1321</v>
       </c>
       <c r="S51" t="s">
-        <v>1364</v>
+        <v>1353</v>
       </c>
       <c r="T51" t="s">
-        <v>1320</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="52" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -7638,13 +7629,13 @@
         <v>44992</v>
       </c>
       <c r="Q52" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="R52" t="s">
-        <v>1330</v>
+        <v>1322</v>
       </c>
       <c r="S52" t="s">
-        <v>1408</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="53" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -7691,13 +7682,13 @@
         <v>44992</v>
       </c>
       <c r="Q53" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="R53" t="s">
-        <v>1331</v>
+        <v>1323</v>
       </c>
       <c r="S53" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="54" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -7741,7 +7732,7 @@
         <v>44992</v>
       </c>
       <c r="Q54" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R54" t="s">
         <v>430</v>
@@ -7797,13 +7788,13 @@
         <v>44992</v>
       </c>
       <c r="Q55" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="R55" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="S55" t="s">
-        <v>1409</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="56" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -7853,13 +7844,13 @@
         <v>44992</v>
       </c>
       <c r="Q56" t="s">
-        <v>1225</v>
+        <v>430</v>
       </c>
       <c r="R56" t="s">
-        <v>1225</v>
+        <v>430</v>
       </c>
       <c r="S56" t="s">
-        <v>1225</v>
+        <v>430</v>
       </c>
     </row>
     <row r="57" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -7906,13 +7897,13 @@
         <v>44992</v>
       </c>
       <c r="Q57" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="R57" t="s">
-        <v>1332</v>
+        <v>1468</v>
       </c>
       <c r="S57" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="58" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -7955,20 +7946,23 @@
       <c r="N58" t="s">
         <v>838</v>
       </c>
+      <c r="O58" t="s">
+        <v>1476</v>
+      </c>
       <c r="P58" s="4">
         <v>44992</v>
       </c>
       <c r="Q58" t="s">
-        <v>1468</v>
+        <v>1474</v>
       </c>
       <c r="R58" t="s">
-        <v>1333</v>
+        <v>1324</v>
       </c>
       <c r="S58" t="s">
-        <v>1410</v>
+        <v>1399</v>
       </c>
       <c r="T58" t="s">
-        <v>1464</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="59" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -8015,13 +8009,13 @@
         <v>44992</v>
       </c>
       <c r="Q59" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="R59" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="S59" t="s">
-        <v>1411</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="60" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -8068,13 +8062,13 @@
         <v>44992</v>
       </c>
       <c r="Q60" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="R60" t="s">
-        <v>1321</v>
+        <v>1316</v>
       </c>
       <c r="S60" t="s">
-        <v>1412</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="61" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -8121,13 +8115,13 @@
         <v>44992</v>
       </c>
       <c r="Q61" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
       <c r="R61" t="s">
-        <v>1334</v>
+        <v>1273</v>
       </c>
       <c r="S61" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="62" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -8170,20 +8164,23 @@
       <c r="N62" t="s">
         <v>842</v>
       </c>
+      <c r="O62" t="s">
+        <v>1475</v>
+      </c>
       <c r="P62" s="4">
         <v>44992</v>
       </c>
       <c r="Q62" t="s">
-        <v>1413</v>
+        <v>1402</v>
       </c>
       <c r="R62" t="s">
-        <v>1335</v>
+        <v>1325</v>
       </c>
       <c r="S62" t="s">
-        <v>1414</v>
+        <v>1403</v>
       </c>
       <c r="T62" t="s">
-        <v>1464</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="63" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -8230,16 +8227,16 @@
         <v>44992</v>
       </c>
       <c r="Q63" t="s">
-        <v>1336</v>
+        <v>1326</v>
       </c>
       <c r="R63" t="s">
-        <v>1336</v>
+        <v>1326</v>
       </c>
       <c r="S63" t="s">
-        <v>1415</v>
+        <v>1404</v>
       </c>
       <c r="T63" t="s">
-        <v>1320</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="64" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -8282,20 +8279,23 @@
       <c r="N64" t="s">
         <v>844</v>
       </c>
+      <c r="O64" t="s">
+        <v>1469</v>
+      </c>
       <c r="P64" s="4">
         <v>44992</v>
       </c>
       <c r="Q64" t="s">
-        <v>1416</v>
+        <v>1405</v>
       </c>
       <c r="R64" t="s">
-        <v>1337</v>
+        <v>1215</v>
       </c>
       <c r="S64" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="T64" t="s">
-        <v>1320</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="65" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -8324,7 +8324,7 @@
         <v>2011</v>
       </c>
       <c r="J65" s="2" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="K65">
         <v>2</v>
@@ -8342,13 +8342,13 @@
         <v>44992</v>
       </c>
       <c r="Q65" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
       <c r="R65" t="s">
-        <v>1338</v>
+        <v>1327</v>
       </c>
       <c r="S65" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="66" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -8392,7 +8392,7 @@
         <v>44992</v>
       </c>
       <c r="Q66" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="R66" t="s">
         <v>430</v>
@@ -8442,7 +8442,7 @@
         <v>44992</v>
       </c>
       <c r="Q67" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="R67" t="s">
         <v>430</v>
@@ -8495,13 +8495,13 @@
         <v>44992</v>
       </c>
       <c r="Q68" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
       <c r="R68" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="S68" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="69" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -8548,13 +8548,13 @@
         <v>44992</v>
       </c>
       <c r="Q69" t="s">
-        <v>1417</v>
+        <v>1406</v>
       </c>
       <c r="R69" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="S69" t="s">
-        <v>1418</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="70" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -8601,13 +8601,13 @@
         <v>44992</v>
       </c>
       <c r="Q70" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="R70" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="S70" t="s">
-        <v>1419</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="71" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -8651,13 +8651,13 @@
         <v>44992</v>
       </c>
       <c r="Q71" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="R71" t="s">
-        <v>479</v>
+        <v>430</v>
       </c>
       <c r="S71" t="s">
-        <v>479</v>
+        <v>430</v>
       </c>
     </row>
     <row r="72" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -8704,13 +8704,13 @@
         <v>44992</v>
       </c>
       <c r="Q72" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="R72" t="s">
-        <v>1339</v>
+        <v>1328</v>
       </c>
       <c r="S72" t="s">
-        <v>1420</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="73" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -8754,7 +8754,7 @@
         <v>44992</v>
       </c>
       <c r="Q73" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="R73" t="s">
         <v>430</v>
@@ -8807,13 +8807,13 @@
         <v>44992</v>
       </c>
       <c r="Q74" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="R74" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="S74" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="75" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -8857,7 +8857,7 @@
         <v>44992</v>
       </c>
       <c r="Q75" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="R75" t="s">
         <v>430</v>
@@ -8910,13 +8910,13 @@
         <v>44992</v>
       </c>
       <c r="Q76" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="R76" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="S76" t="s">
-        <v>1363</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="77" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -8963,13 +8963,13 @@
         <v>44992</v>
       </c>
       <c r="Q77" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="R77" t="s">
-        <v>1340</v>
+        <v>1329</v>
       </c>
       <c r="S77" t="s">
-        <v>1421</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="78" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -9016,13 +9016,13 @@
         <v>44992</v>
       </c>
       <c r="Q78" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="R78" t="s">
-        <v>1341</v>
+        <v>1330</v>
       </c>
       <c r="S78" t="s">
-        <v>1422</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="79" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -9069,13 +9069,13 @@
         <v>45012</v>
       </c>
       <c r="Q79" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
       <c r="R79" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="S79" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="80" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -9122,13 +9122,13 @@
         <v>45012</v>
       </c>
       <c r="Q80" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="R80" t="s">
-        <v>1342</v>
+        <v>1331</v>
       </c>
       <c r="S80" t="s">
-        <v>1423</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="81" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -9175,13 +9175,13 @@
         <v>45012</v>
       </c>
       <c r="Q81" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="R81" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="S81" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="82" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -9225,7 +9225,7 @@
         <v>45012</v>
       </c>
       <c r="Q82" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R82" t="s">
         <v>430</v>
@@ -9275,7 +9275,7 @@
         <v>45012</v>
       </c>
       <c r="Q83" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="R83" t="s">
         <v>430</v>
@@ -9325,7 +9325,7 @@
         <v>45012</v>
       </c>
       <c r="Q84" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="R84" t="s">
         <v>430</v>
@@ -9378,13 +9378,13 @@
         <v>45012</v>
       </c>
       <c r="Q85" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="R85" t="s">
-        <v>1469</v>
+        <v>1456</v>
       </c>
       <c r="S85" t="s">
-        <v>1424</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="86" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -9431,13 +9431,13 @@
         <v>45012</v>
       </c>
       <c r="Q86" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="R86" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="S86" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="87" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -9484,13 +9484,13 @@
         <v>45012</v>
       </c>
       <c r="Q87" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="R87" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="S87" t="s">
-        <v>1425</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="88" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -9534,7 +9534,7 @@
         <v>45012</v>
       </c>
       <c r="Q88" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="R88" t="s">
         <v>430</v>
@@ -9557,7 +9557,7 @@
         <v>2016</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>1349</v>
+        <v>1338</v>
       </c>
       <c r="G89">
         <v>2018</v>
@@ -9587,13 +9587,13 @@
         <v>45012</v>
       </c>
       <c r="Q89" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="R89" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="S89" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="90" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -9640,13 +9640,13 @@
         <v>45012</v>
       </c>
       <c r="Q90" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="R90" t="s">
-        <v>1343</v>
+        <v>1332</v>
       </c>
       <c r="S90" t="s">
-        <v>1426</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="91" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -9693,13 +9693,13 @@
         <v>45012</v>
       </c>
       <c r="Q91" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="R91" t="s">
-        <v>1344</v>
+        <v>1333</v>
       </c>
       <c r="S91" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="92" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -9743,7 +9743,7 @@
         <v>45012</v>
       </c>
       <c r="Q92" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="R92" t="s">
         <v>430</v>
@@ -9843,7 +9843,7 @@
         <v>45012</v>
       </c>
       <c r="Q94" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R94" t="s">
         <v>430</v>
@@ -9893,7 +9893,7 @@
         <v>45012</v>
       </c>
       <c r="Q95" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="R95" t="s">
         <v>430</v>
@@ -9946,13 +9946,13 @@
         <v>45012</v>
       </c>
       <c r="Q96" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="R96" t="s">
-        <v>1345</v>
+        <v>1334</v>
       </c>
       <c r="S96" t="s">
-        <v>1400</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="97" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -9999,16 +9999,16 @@
         <v>45012</v>
       </c>
       <c r="Q97" t="s">
-        <v>1372</v>
+        <v>1361</v>
       </c>
       <c r="R97" t="s">
         <v>1206</v>
       </c>
       <c r="S97" t="s">
-        <v>1372</v>
+        <v>1361</v>
       </c>
       <c r="T97" t="s">
-        <v>1320</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="98" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -10052,13 +10052,13 @@
         <v>45012</v>
       </c>
       <c r="Q98" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="R98" t="s">
-        <v>449</v>
+        <v>430</v>
       </c>
       <c r="S98" t="s">
-        <v>449</v>
+        <v>430</v>
       </c>
     </row>
     <row r="99" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -10105,16 +10105,16 @@
         <v>45012</v>
       </c>
       <c r="Q99" t="s">
-        <v>1346</v>
+        <v>1335</v>
       </c>
       <c r="R99" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="S99" t="s">
-        <v>1427</v>
+        <v>1416</v>
       </c>
       <c r="T99" t="s">
-        <v>1464</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="100" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -10161,13 +10161,13 @@
         <v>45012</v>
       </c>
       <c r="Q100" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="R100" t="s">
-        <v>1347</v>
+        <v>1336</v>
       </c>
       <c r="S100" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="101" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -10214,13 +10214,13 @@
         <v>45012</v>
       </c>
       <c r="Q101" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="R101" t="s">
-        <v>1348</v>
+        <v>1337</v>
       </c>
       <c r="S101" t="s">
-        <v>1397</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="102" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -10264,7 +10264,7 @@
         <v>45012</v>
       </c>
       <c r="Q102" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R102" t="s">
         <v>430</v>
@@ -10314,7 +10314,7 @@
         <v>45012</v>
       </c>
       <c r="Q103" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R103" t="s">
         <v>430</v>
@@ -10367,13 +10367,13 @@
         <v>45012</v>
       </c>
       <c r="Q104" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="R104" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="S104" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="105" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -10417,7 +10417,7 @@
         <v>45012</v>
       </c>
       <c r="Q105" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R105" t="s">
         <v>430</v>
@@ -10470,13 +10470,13 @@
         <v>45012</v>
       </c>
       <c r="Q106" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="R106" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="S106" t="s">
-        <v>1428</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="107" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -10523,13 +10523,13 @@
         <v>45012</v>
       </c>
       <c r="Q107" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R107" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="S107" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="108" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -10573,7 +10573,7 @@
         <v>45012</v>
       </c>
       <c r="Q108" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R108" t="s">
         <v>430</v>
@@ -10626,13 +10626,13 @@
         <v>45012</v>
       </c>
       <c r="Q109" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
       <c r="R109" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="S109" t="s">
-        <v>1429</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="110" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -10679,13 +10679,13 @@
         <v>45012</v>
       </c>
       <c r="Q110" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="R110" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="S110" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="111" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -10729,7 +10729,7 @@
         <v>45012</v>
       </c>
       <c r="Q111" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R111" t="s">
         <v>430</v>
@@ -10779,7 +10779,7 @@
         <v>45012</v>
       </c>
       <c r="Q112" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R112" t="s">
         <v>430</v>
@@ -10832,13 +10832,13 @@
         <v>45012</v>
       </c>
       <c r="Q113" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
       <c r="R113" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="S113" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="114" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -10885,13 +10885,13 @@
         <v>45012</v>
       </c>
       <c r="Q114" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R114" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="S114" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="115" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -10938,7 +10938,7 @@
         <v>45012</v>
       </c>
       <c r="Q115" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R115" t="s">
         <v>430</v>
@@ -10991,7 +10991,7 @@
         <v>45012</v>
       </c>
       <c r="Q116" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R116" t="s">
         <v>430</v>
@@ -11044,13 +11044,13 @@
         <v>45012</v>
       </c>
       <c r="Q117" t="s">
-        <v>1430</v>
+        <v>1419</v>
       </c>
       <c r="R117" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="S117" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="118" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -11097,16 +11097,16 @@
         <v>45012</v>
       </c>
       <c r="Q118" t="s">
-        <v>1350</v>
+        <v>1339</v>
       </c>
       <c r="R118" t="s">
-        <v>1351</v>
+        <v>1340</v>
       </c>
       <c r="S118" t="s">
-        <v>1397</v>
+        <v>1386</v>
       </c>
       <c r="T118" t="s">
-        <v>1464</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="119" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -11153,13 +11153,13 @@
         <v>45012</v>
       </c>
       <c r="Q119" t="s">
-        <v>1353</v>
+        <v>1342</v>
       </c>
       <c r="R119" t="s">
-        <v>1352</v>
+        <v>1341</v>
       </c>
       <c r="S119" t="s">
-        <v>1431</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="120" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -11206,13 +11206,13 @@
         <v>45012</v>
       </c>
       <c r="Q120" t="s">
-        <v>1470</v>
+        <v>1457</v>
       </c>
       <c r="R120" t="s">
-        <v>1354</v>
+        <v>1343</v>
       </c>
       <c r="S120" t="s">
-        <v>1432</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="121" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -11259,13 +11259,13 @@
         <v>45012</v>
       </c>
       <c r="Q121" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="R121" t="s">
-        <v>479</v>
+        <v>430</v>
       </c>
       <c r="S121" t="s">
-        <v>479</v>
+        <v>430</v>
       </c>
     </row>
     <row r="122" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -11309,16 +11309,16 @@
         <v>45012</v>
       </c>
       <c r="Q122" t="s">
-        <v>1433</v>
+        <v>1422</v>
       </c>
       <c r="R122" t="s">
-        <v>479</v>
+        <v>430</v>
       </c>
       <c r="S122" t="s">
-        <v>479</v>
+        <v>430</v>
       </c>
       <c r="T122" t="s">
-        <v>1464</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="123" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -11362,16 +11362,16 @@
         <v>45012</v>
       </c>
       <c r="Q123" t="s">
-        <v>1434</v>
+        <v>1423</v>
       </c>
       <c r="R123" t="s">
-        <v>479</v>
+        <v>430</v>
       </c>
       <c r="S123" t="s">
-        <v>479</v>
+        <v>430</v>
       </c>
       <c r="T123" t="s">
-        <v>1464</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="124" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -11418,7 +11418,7 @@
         <v>45012</v>
       </c>
       <c r="Q124" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R124" t="s">
         <v>430</v>
@@ -11471,13 +11471,13 @@
         <v>45012</v>
       </c>
       <c r="Q125" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="R125" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="S125" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="126" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -11524,13 +11524,13 @@
         <v>45012</v>
       </c>
       <c r="Q126" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
       <c r="R126" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="S126" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="127" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -11574,7 +11574,7 @@
         <v>45012</v>
       </c>
       <c r="Q127" t="s">
-        <v>1400</v>
+        <v>1389</v>
       </c>
       <c r="R127" t="s">
         <v>430</v>
@@ -11624,7 +11624,7 @@
         <v>45012</v>
       </c>
       <c r="Q128" t="s">
-        <v>1355</v>
+        <v>1344</v>
       </c>
       <c r="R128" t="s">
         <v>430</v>
@@ -11677,13 +11677,13 @@
         <v>45012</v>
       </c>
       <c r="Q129" t="s">
-        <v>1471</v>
+        <v>1458</v>
       </c>
       <c r="R129" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="S129" t="s">
-        <v>1435</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="130" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -11730,13 +11730,13 @@
         <v>45012</v>
       </c>
       <c r="Q130" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="R130" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="S130" t="s">
-        <v>1436</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="131" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -11783,13 +11783,13 @@
         <v>45012</v>
       </c>
       <c r="Q131" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="R131" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="S131" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="132" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -11833,7 +11833,7 @@
         <v>45012</v>
       </c>
       <c r="Q132" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="R132" t="s">
         <v>430</v>
@@ -11883,7 +11883,7 @@
         <v>45012</v>
       </c>
       <c r="Q133" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="R133" t="s">
         <v>430</v>
@@ -11936,7 +11936,7 @@
         <v>45012</v>
       </c>
       <c r="Q134" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="R134" t="s">
         <v>430</v>
@@ -11989,13 +11989,13 @@
         <v>45034</v>
       </c>
       <c r="Q135" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
       <c r="R135" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="S135" t="s">
-        <v>1437</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="136" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -12042,13 +12042,13 @@
         <v>45034</v>
       </c>
       <c r="Q136" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
       <c r="R136" t="s">
-        <v>1356</v>
+        <v>1345</v>
       </c>
       <c r="S136" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="137" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -12095,13 +12095,13 @@
         <v>45034</v>
       </c>
       <c r="Q137" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="R137" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="S137" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="138" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -12145,7 +12145,7 @@
         <v>45034</v>
       </c>
       <c r="Q138" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="R138" t="s">
         <v>430</v>
@@ -12198,13 +12198,13 @@
         <v>45034</v>
       </c>
       <c r="Q139" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="R139" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="S139" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="140" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -12251,13 +12251,13 @@
         <v>45034</v>
       </c>
       <c r="Q140" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="R140" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="S140" t="s">
-        <v>1438</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="141" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -12304,16 +12304,16 @@
         <v>45034</v>
       </c>
       <c r="Q141" t="s">
-        <v>1439</v>
+        <v>1428</v>
       </c>
       <c r="R141" t="s">
-        <v>1357</v>
+        <v>1346</v>
       </c>
       <c r="S141" t="s">
-        <v>1440</v>
+        <v>1429</v>
       </c>
       <c r="T141" t="s">
-        <v>1320</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="142" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -12357,7 +12357,7 @@
         <v>45034</v>
       </c>
       <c r="Q142" t="s">
-        <v>1472</v>
+        <v>1459</v>
       </c>
       <c r="R142" t="s">
         <v>430</v>
@@ -12407,7 +12407,7 @@
         <v>45034</v>
       </c>
       <c r="Q143" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R143" t="s">
         <v>430</v>
@@ -12460,13 +12460,13 @@
         <v>45034</v>
       </c>
       <c r="Q144" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
       <c r="R144" t="s">
-        <v>1321</v>
+        <v>1316</v>
       </c>
       <c r="S144" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="145" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -12510,7 +12510,7 @@
         <v>45034</v>
       </c>
       <c r="Q145" t="s">
-        <v>1473</v>
+        <v>1460</v>
       </c>
       <c r="R145" t="s">
         <v>430</v>
@@ -12563,16 +12563,16 @@
         <v>45034</v>
       </c>
       <c r="Q146" t="s">
-        <v>1358</v>
+        <v>1347</v>
       </c>
       <c r="R146" t="s">
-        <v>1358</v>
+        <v>1347</v>
       </c>
       <c r="S146" t="s">
-        <v>1358</v>
+        <v>1347</v>
       </c>
       <c r="T146" t="s">
-        <v>1320</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="147" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -12619,7 +12619,7 @@
         <v>45034</v>
       </c>
       <c r="Q147" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="R147" t="s">
         <v>430</v>
@@ -12672,7 +12672,7 @@
         <v>45034</v>
       </c>
       <c r="Q148" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="R148" t="s">
         <v>430</v>
@@ -12725,7 +12725,7 @@
         <v>45034</v>
       </c>
       <c r="Q149" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="R149" t="s">
         <v>430</v>
@@ -12778,7 +12778,7 @@
         <v>45034</v>
       </c>
       <c r="Q150" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="R150" t="s">
         <v>430</v>
@@ -12831,13 +12831,13 @@
         <v>45034</v>
       </c>
       <c r="Q151" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="R151" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="S151" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="152" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -12884,13 +12884,13 @@
         <v>45034</v>
       </c>
       <c r="Q152" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="R152" t="s">
-        <v>1359</v>
+        <v>1348</v>
       </c>
       <c r="S152" t="s">
-        <v>1400</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="153" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -12937,13 +12937,13 @@
         <v>45034</v>
       </c>
       <c r="Q153" t="s">
-        <v>1441</v>
+        <v>1430</v>
       </c>
       <c r="R153" t="s">
-        <v>1360</v>
+        <v>1349</v>
       </c>
       <c r="S153" t="s">
-        <v>1442</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="154" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -12987,7 +12987,7 @@
         <v>45034</v>
       </c>
       <c r="Q154" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R154" t="s">
         <v>430</v>
@@ -13037,7 +13037,7 @@
         <v>45034</v>
       </c>
       <c r="Q155" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R155" t="s">
         <v>430</v>
@@ -13090,13 +13090,13 @@
         <v>45034</v>
       </c>
       <c r="Q156" t="s">
-        <v>1474</v>
+        <v>1461</v>
       </c>
       <c r="R156" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="S156" t="s">
-        <v>1443</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="157" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -13140,7 +13140,7 @@
         <v>45034</v>
       </c>
       <c r="Q157" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R157" t="s">
         <v>430</v>
@@ -13193,13 +13193,13 @@
         <v>45034</v>
       </c>
       <c r="Q158" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="R158" t="s">
-        <v>1361</v>
+        <v>1350</v>
       </c>
       <c r="S158" t="s">
-        <v>1444</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="159" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -13243,7 +13243,7 @@
         <v>45034</v>
       </c>
       <c r="Q159" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R159" t="s">
         <v>430</v>
@@ -13296,13 +13296,13 @@
         <v>45034</v>
       </c>
       <c r="Q160" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R160" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="S160" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="161" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -13346,7 +13346,7 @@
         <v>45034</v>
       </c>
       <c r="Q161" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R161" t="s">
         <v>430</v>
@@ -13399,13 +13399,13 @@
         <v>45034</v>
       </c>
       <c r="Q162" t="s">
-        <v>1463</v>
+        <v>1452</v>
       </c>
       <c r="R162" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="S162" t="s">
-        <v>1445</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="163" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -13449,7 +13449,7 @@
         <v>45034</v>
       </c>
       <c r="Q163" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R163" t="s">
         <v>430</v>
@@ -13502,13 +13502,13 @@
         <v>45034</v>
       </c>
       <c r="Q164" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="R164" t="s">
-        <v>1362</v>
+        <v>1351</v>
       </c>
       <c r="S164" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="165" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -13552,7 +13552,7 @@
         <v>45034</v>
       </c>
       <c r="Q165" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R165" t="s">
         <v>430</v>
@@ -13605,13 +13605,13 @@
         <v>45034</v>
       </c>
       <c r="Q166" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="R166" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="S166" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="167" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -13658,13 +13658,13 @@
         <v>45034</v>
       </c>
       <c r="Q167" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="R167" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="S167" t="s">
-        <v>1367</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="168" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -13711,13 +13711,13 @@
         <v>45034</v>
       </c>
       <c r="Q168" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="R168" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="S168" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="169" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -13764,13 +13764,13 @@
         <v>45034</v>
       </c>
       <c r="Q169" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="R169" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="S169" t="s">
-        <v>1446</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="170" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -13814,7 +13814,7 @@
         <v>45034</v>
       </c>
       <c r="Q170" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R170" t="s">
         <v>430</v>
@@ -13867,13 +13867,13 @@
         <v>45034</v>
       </c>
       <c r="Q171" t="s">
-        <v>1364</v>
+        <v>1353</v>
       </c>
       <c r="R171" t="s">
-        <v>1363</v>
+        <v>1352</v>
       </c>
       <c r="S171" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="172" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -13920,13 +13920,13 @@
         <v>45034</v>
       </c>
       <c r="Q172" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="R172" t="s">
-        <v>479</v>
+        <v>430</v>
       </c>
       <c r="S172" t="s">
-        <v>479</v>
+        <v>430</v>
       </c>
     </row>
     <row r="173" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -13973,13 +13973,13 @@
         <v>45034</v>
       </c>
       <c r="Q173" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="R173" t="s">
-        <v>479</v>
+        <v>430</v>
       </c>
       <c r="S173" t="s">
-        <v>479</v>
+        <v>430</v>
       </c>
     </row>
     <row r="174" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -14020,22 +14020,22 @@
         <v>951</v>
       </c>
       <c r="O174" t="s">
-        <v>1045</v>
+        <v>1464</v>
       </c>
       <c r="P174" s="4">
         <v>45034</v>
       </c>
       <c r="Q174" t="s">
-        <v>1217</v>
+        <v>1454</v>
       </c>
       <c r="R174" t="s">
-        <v>479</v>
+        <v>430</v>
       </c>
       <c r="S174" t="s">
-        <v>479</v>
+        <v>430</v>
       </c>
       <c r="T174" t="s">
-        <v>1464</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="175" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -14082,16 +14082,16 @@
         <v>45034</v>
       </c>
       <c r="Q175" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R175" t="s">
-        <v>479</v>
+        <v>430</v>
       </c>
       <c r="S175" t="s">
-        <v>479</v>
+        <v>430</v>
       </c>
       <c r="T175" t="s">
-        <v>1464</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="176" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -14141,13 +14141,13 @@
         <v>45034</v>
       </c>
       <c r="Q176" t="s">
+        <v>1271</v>
+      </c>
+      <c r="R176" t="s">
         <v>1273</v>
       </c>
-      <c r="R176" t="s">
-        <v>1275</v>
-      </c>
       <c r="S176" t="s">
-        <v>1429</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="177" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -14191,7 +14191,7 @@
         <v>45034</v>
       </c>
       <c r="Q177" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R177" t="s">
         <v>430</v>
@@ -14241,7 +14241,7 @@
         <v>45034</v>
       </c>
       <c r="Q178" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="R178" t="s">
         <v>430</v>
@@ -14294,13 +14294,13 @@
         <v>45034</v>
       </c>
       <c r="Q179" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="R179" t="s">
-        <v>1365</v>
+        <v>1354</v>
       </c>
       <c r="S179" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="180" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -14344,7 +14344,7 @@
         <v>45034</v>
       </c>
       <c r="Q180" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="R180" t="s">
         <v>430</v>
@@ -14397,13 +14397,13 @@
         <v>45034</v>
       </c>
       <c r="Q181" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="R181" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="S181" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="182" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -14447,7 +14447,7 @@
         <v>45034</v>
       </c>
       <c r="Q182" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="R182" t="s">
         <v>430</v>
@@ -14497,7 +14497,7 @@
         <v>45034</v>
       </c>
       <c r="Q183" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="R183" t="s">
         <v>430</v>
@@ -14547,7 +14547,7 @@
         <v>45034</v>
       </c>
       <c r="Q184" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="R184" t="s">
         <v>430</v>
@@ -14597,7 +14597,7 @@
         <v>45034</v>
       </c>
       <c r="Q185" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R185" t="s">
         <v>430</v>
@@ -14647,7 +14647,7 @@
         <v>45034</v>
       </c>
       <c r="Q186" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="R186" t="s">
         <v>430</v>
@@ -14697,7 +14697,7 @@
         <v>45034</v>
       </c>
       <c r="Q187" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="R187" t="s">
         <v>430</v>
@@ -14747,13 +14747,13 @@
         <v>45012</v>
       </c>
       <c r="Q188" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R188" t="s">
-        <v>479</v>
+        <v>430</v>
       </c>
       <c r="S188" t="s">
-        <v>479</v>
+        <v>430</v>
       </c>
     </row>
     <row r="189" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -14797,7 +14797,7 @@
         <v>45012</v>
       </c>
       <c r="Q189" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R189" t="s">
         <v>430</v>
@@ -14850,13 +14850,13 @@
         <v>45012</v>
       </c>
       <c r="Q190" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
       <c r="R190" t="s">
-        <v>1321</v>
+        <v>1316</v>
       </c>
       <c r="S190" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="191" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -14903,13 +14903,13 @@
         <v>45012</v>
       </c>
       <c r="Q191" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="R191" t="s">
-        <v>1366</v>
+        <v>1355</v>
       </c>
       <c r="S191" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="192" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -14953,7 +14953,7 @@
         <v>45012</v>
       </c>
       <c r="Q192" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R192" t="s">
         <v>430</v>
@@ -15003,7 +15003,7 @@
         <v>45034</v>
       </c>
       <c r="Q193" t="s">
-        <v>1477</v>
+        <v>1463</v>
       </c>
       <c r="R193" t="s">
         <v>430</v>
@@ -15053,7 +15053,7 @@
         <v>45034</v>
       </c>
       <c r="Q194" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R194" t="s">
         <v>430</v>
@@ -15106,13 +15106,13 @@
         <v>45034</v>
       </c>
       <c r="Q195" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="R195" t="s">
-        <v>1347</v>
+        <v>1336</v>
       </c>
       <c r="S195" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="196" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -15159,13 +15159,13 @@
         <v>45034</v>
       </c>
       <c r="Q196" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="R196" t="s">
-        <v>1367</v>
+        <v>1356</v>
       </c>
       <c r="S196" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="197" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -15212,13 +15212,13 @@
         <v>45034</v>
       </c>
       <c r="Q197" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="R197" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="S197" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="198" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -15265,13 +15265,13 @@
         <v>45034</v>
       </c>
       <c r="Q198" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
       <c r="R198" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="S198" t="s">
-        <v>1447</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="199" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -15318,16 +15318,16 @@
         <v>45034</v>
       </c>
       <c r="Q199" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="R199" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="S199" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="T199" t="s">
-        <v>1320</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="200" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -15371,7 +15371,7 @@
         <v>45034</v>
       </c>
       <c r="Q200" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R200" t="s">
         <v>430</v>
@@ -15424,13 +15424,13 @@
         <v>45034</v>
       </c>
       <c r="Q201" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
       <c r="R201" t="s">
-        <v>1368</v>
+        <v>1357</v>
       </c>
       <c r="S201" t="s">
-        <v>1347</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="202" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -15474,7 +15474,7 @@
         <v>45034</v>
       </c>
       <c r="Q202" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
       <c r="R202" t="s">
         <v>430</v>
@@ -15524,13 +15524,13 @@
         <v>45034</v>
       </c>
       <c r="Q203" t="s">
-        <v>1283</v>
+        <v>1281</v>
       </c>
       <c r="R203" t="s">
-        <v>479</v>
+        <v>430</v>
       </c>
       <c r="S203" t="s">
-        <v>479</v>
+        <v>430</v>
       </c>
     </row>
     <row r="204" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -15574,7 +15574,7 @@
         <v>45034</v>
       </c>
       <c r="Q204" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R204" t="s">
         <v>430</v>
@@ -15627,13 +15627,13 @@
         <v>45034</v>
       </c>
       <c r="Q205" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="R205" t="s">
-        <v>1344</v>
+        <v>1333</v>
       </c>
       <c r="S205" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="206" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -15677,13 +15677,13 @@
         <v>45034</v>
       </c>
       <c r="Q206" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="R206" t="s">
-        <v>449</v>
+        <v>430</v>
       </c>
       <c r="S206" t="s">
-        <v>449</v>
+        <v>430</v>
       </c>
     </row>
     <row r="207" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -15727,7 +15727,7 @@
         <v>45034</v>
       </c>
       <c r="Q207" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R207" t="s">
         <v>430</v>
@@ -15780,16 +15780,16 @@
         <v>45034</v>
       </c>
       <c r="Q208" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
       <c r="R208" t="s">
-        <v>1369</v>
+        <v>1358</v>
       </c>
       <c r="S208" t="s">
-        <v>1448</v>
+        <v>1437</v>
       </c>
       <c r="T208" t="s">
-        <v>1320</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="209" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -15836,13 +15836,13 @@
         <v>45034</v>
       </c>
       <c r="Q209" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="R209" t="s">
-        <v>1370</v>
+        <v>1359</v>
       </c>
       <c r="S209" t="s">
-        <v>1449</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="210" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -15886,7 +15886,7 @@
         <v>45034</v>
       </c>
       <c r="Q210" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R210" t="s">
         <v>430</v>
@@ -15939,13 +15939,13 @@
         <v>45034</v>
       </c>
       <c r="Q211" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="R211" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="S211" t="s">
-        <v>1390</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="212" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -15992,13 +15992,13 @@
         <v>45034</v>
       </c>
       <c r="Q212" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="R212" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="S212" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="213" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -16045,13 +16045,13 @@
         <v>45034</v>
       </c>
       <c r="Q213" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
       <c r="R213" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="S213" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="214" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -16098,13 +16098,13 @@
         <v>45034</v>
       </c>
       <c r="Q214" t="s">
-        <v>1372</v>
+        <v>1361</v>
       </c>
       <c r="R214" t="s">
-        <v>1371</v>
+        <v>1360</v>
       </c>
       <c r="S214" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="215" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -16151,13 +16151,13 @@
         <v>45012</v>
       </c>
       <c r="Q215" t="s">
-        <v>1373</v>
+        <v>1362</v>
       </c>
       <c r="R215" t="s">
-        <v>1374</v>
+        <v>1363</v>
       </c>
       <c r="S215" t="s">
-        <v>1450</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="216" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -16204,13 +16204,13 @@
         <v>45012</v>
       </c>
       <c r="Q216" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
       <c r="R216" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="S216" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="217" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -16257,13 +16257,13 @@
         <v>45012</v>
       </c>
       <c r="Q217" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="R217" t="s">
-        <v>1375</v>
+        <v>1364</v>
       </c>
       <c r="S217" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="218" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -16307,7 +16307,7 @@
         <v>45012</v>
       </c>
       <c r="Q218" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R218" t="s">
         <v>430</v>
@@ -16360,13 +16360,13 @@
         <v>45012</v>
       </c>
       <c r="Q219" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="R219" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="S219" t="s">
-        <v>1400</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="220" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -16410,7 +16410,7 @@
         <v>45012</v>
       </c>
       <c r="Q220" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R220" t="s">
         <v>430</v>
@@ -16463,13 +16463,13 @@
         <v>45012</v>
       </c>
       <c r="Q221" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="R221" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="S221" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="222" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -16513,7 +16513,7 @@
         <v>45012</v>
       </c>
       <c r="Q222" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R222" t="s">
         <v>430</v>
@@ -16566,13 +16566,13 @@
         <v>45012</v>
       </c>
       <c r="Q223" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
       <c r="R223" t="s">
-        <v>1376</v>
+        <v>1365</v>
       </c>
       <c r="S223" t="s">
-        <v>1451</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="224" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -16616,7 +16616,7 @@
         <v>45012</v>
       </c>
       <c r="Q224" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="R224" t="s">
         <v>430</v>
@@ -16669,13 +16669,13 @@
         <v>45012</v>
       </c>
       <c r="Q225" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="R225" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="S225" t="s">
-        <v>1452</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="226" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -16719,7 +16719,7 @@
         <v>45012</v>
       </c>
       <c r="Q226" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="R226" t="s">
         <v>430</v>
@@ -16769,7 +16769,7 @@
         <v>45012</v>
       </c>
       <c r="Q227" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R227" t="s">
         <v>430</v>
@@ -16819,7 +16819,7 @@
         <v>45012</v>
       </c>
       <c r="Q228" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R228" t="s">
         <v>430</v>
@@ -16869,7 +16869,7 @@
         <v>45012</v>
       </c>
       <c r="Q229" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="R229" t="s">
         <v>430</v>
@@ -16922,13 +16922,13 @@
         <v>45012</v>
       </c>
       <c r="Q230" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
       <c r="R230" t="s">
-        <v>1347</v>
+        <v>1336</v>
       </c>
       <c r="S230" t="s">
-        <v>1453</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="231" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -16975,13 +16975,13 @@
         <v>45012</v>
       </c>
       <c r="Q231" t="s">
-        <v>1378</v>
+        <v>1367</v>
       </c>
       <c r="R231" t="s">
-        <v>1377</v>
+        <v>1366</v>
       </c>
       <c r="S231" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="232" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -17028,16 +17028,16 @@
         <v>45012</v>
       </c>
       <c r="Q232" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="R232" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="S232" t="s">
-        <v>1347</v>
+        <v>1336</v>
       </c>
       <c r="T232" t="s">
-        <v>1320</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="233" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -17084,13 +17084,13 @@
         <v>45012</v>
       </c>
       <c r="Q233" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="R233" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="S233" t="s">
-        <v>1454</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="234" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -17137,13 +17137,13 @@
         <v>45012</v>
       </c>
       <c r="Q234" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
       <c r="R234" t="s">
-        <v>1379</v>
+        <v>1368</v>
       </c>
       <c r="S234" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="235" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -17190,13 +17190,13 @@
         <v>45012</v>
       </c>
       <c r="Q235" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
       <c r="R235" t="s">
-        <v>1338</v>
+        <v>1327</v>
       </c>
       <c r="S235" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="236" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -17243,13 +17243,13 @@
         <v>45012</v>
       </c>
       <c r="Q236" t="s">
-        <v>1380</v>
+        <v>1369</v>
       </c>
       <c r="R236" t="s">
-        <v>1381</v>
+        <v>1370</v>
       </c>
       <c r="S236" t="s">
-        <v>1400</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="237" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -17293,7 +17293,7 @@
         <v>45012</v>
       </c>
       <c r="Q237" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="R237" t="s">
         <v>430</v>
@@ -17346,13 +17346,13 @@
         <v>45012</v>
       </c>
       <c r="Q238" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="R238" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="S238" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="239" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -17399,13 +17399,13 @@
         <v>45012</v>
       </c>
       <c r="Q239" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
       <c r="R239" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="S239" t="s">
-        <v>1447</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="240" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -17452,13 +17452,13 @@
         <v>45012</v>
       </c>
       <c r="Q240" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="R240" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="S240" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="241" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -17502,7 +17502,7 @@
         <v>45012</v>
       </c>
       <c r="Q241" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R241" t="s">
         <v>430</v>
@@ -17555,13 +17555,13 @@
         <v>45012</v>
       </c>
       <c r="Q242" t="s">
-        <v>1475</v>
+        <v>1462</v>
       </c>
       <c r="R242" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="S242" t="s">
-        <v>1455</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="243" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -17605,7 +17605,7 @@
         <v>45012</v>
       </c>
       <c r="Q243" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R243" t="s">
         <v>430</v>
@@ -17658,13 +17658,13 @@
         <v>45012</v>
       </c>
       <c r="Q244" t="s">
-        <v>1299</v>
+        <v>1297</v>
       </c>
       <c r="R244" t="s">
-        <v>1382</v>
+        <v>1371</v>
       </c>
       <c r="S244" t="s">
-        <v>1408</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="245" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -17708,13 +17708,13 @@
         <v>45012</v>
       </c>
       <c r="Q245" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="R245" t="s">
-        <v>479</v>
+        <v>430</v>
       </c>
       <c r="S245" t="s">
-        <v>479</v>
+        <v>430</v>
       </c>
     </row>
     <row r="246" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -17761,13 +17761,13 @@
         <v>45012</v>
       </c>
       <c r="Q246" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="R246" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="S246" t="s">
-        <v>1456</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="247" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -17814,13 +17814,13 @@
         <v>45012</v>
       </c>
       <c r="Q247" t="s">
-        <v>1300</v>
+        <v>1298</v>
       </c>
       <c r="R247" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="S247" t="s">
-        <v>1457</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="248" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -17867,13 +17867,13 @@
         <v>45012</v>
       </c>
       <c r="Q248" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
       <c r="R248" t="s">
-        <v>1347</v>
+        <v>1336</v>
       </c>
       <c r="S248" t="s">
-        <v>1458</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="249" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -17920,13 +17920,13 @@
         <v>45012</v>
       </c>
       <c r="Q249" t="s">
-        <v>1383</v>
+        <v>1372</v>
       </c>
       <c r="R249" t="s">
-        <v>1384</v>
+        <v>1373</v>
       </c>
       <c r="S249" t="s">
-        <v>1459</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="250" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -17973,13 +17973,13 @@
         <v>45012</v>
       </c>
       <c r="Q250" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="R250" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="S250" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="251" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -18023,7 +18023,7 @@
         <v>45012</v>
       </c>
       <c r="Q251" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R251" t="s">
         <v>430</v>
@@ -18076,13 +18076,13 @@
         <v>45012</v>
       </c>
       <c r="Q252" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
       <c r="R252" t="s">
         <v>1206</v>
       </c>
       <c r="S252" t="s">
-        <v>1367</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="253" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -18126,7 +18126,7 @@
         <v>45012</v>
       </c>
       <c r="Q253" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="R253" t="s">
         <v>430</v>
@@ -18179,13 +18179,13 @@
         <v>45012</v>
       </c>
       <c r="Q254" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R254" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="S254" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="255" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -18232,13 +18232,13 @@
         <v>45012</v>
       </c>
       <c r="Q255" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="R255" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="S255" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="256" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -18285,13 +18285,13 @@
         <v>45012</v>
       </c>
       <c r="Q256" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
       <c r="R256" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="S256" t="s">
-        <v>1352</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="257" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -18338,13 +18338,13 @@
         <v>45012</v>
       </c>
       <c r="Q257" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="R257" t="s">
-        <v>1352</v>
+        <v>1341</v>
       </c>
       <c r="S257" t="s">
-        <v>1460</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="258" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -18391,13 +18391,13 @@
         <v>45012</v>
       </c>
       <c r="Q258" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="R258" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="S258" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="259" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -18444,13 +18444,13 @@
         <v>45012</v>
       </c>
       <c r="Q259" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="R259" t="s">
-        <v>1385</v>
+        <v>1374</v>
       </c>
       <c r="S259" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="260" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -18497,13 +18497,13 @@
         <v>45012</v>
       </c>
       <c r="Q260" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
       <c r="R260" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="S260" t="s">
-        <v>1461</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="261" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -18547,7 +18547,7 @@
         <v>45012</v>
       </c>
       <c r="Q261" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="R261" t="s">
         <v>430</v>
@@ -18597,7 +18597,7 @@
         <v>45012</v>
       </c>
       <c r="Q262" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="R262" t="s">
         <v>430</v>
@@ -18650,13 +18650,13 @@
         <v>45012</v>
       </c>
       <c r="Q263" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
       <c r="R263" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="S263" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="264" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -18703,13 +18703,13 @@
         <v>45012</v>
       </c>
       <c r="Q264" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R264" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="S264" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="265" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -18756,13 +18756,13 @@
         <v>45012</v>
       </c>
       <c r="Q265" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
       <c r="R265" t="s">
-        <v>1386</v>
+        <v>1375</v>
       </c>
       <c r="S265" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="266" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -18806,7 +18806,7 @@
         <v>45012</v>
       </c>
       <c r="Q266" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R266" t="s">
         <v>430</v>
@@ -18859,13 +18859,13 @@
         <v>45012</v>
       </c>
       <c r="Q267" t="s">
-        <v>1387</v>
+        <v>1376</v>
       </c>
       <c r="R267" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="S267" t="s">
-        <v>1462</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="268" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -18909,7 +18909,7 @@
         <v>45012</v>
       </c>
       <c r="Q268" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R268" t="s">
         <v>430</v>
@@ -18959,7 +18959,7 @@
         <v>45012</v>
       </c>
       <c r="Q269" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R269" t="s">
         <v>430</v>
@@ -19009,7 +19009,7 @@
         <v>45012</v>
       </c>
       <c r="Q270" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="R270" t="s">
         <v>430</v>
@@ -19062,13 +19062,13 @@
         <v>45012</v>
       </c>
       <c r="Q271" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
       <c r="R271" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="S271" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="272" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -19112,7 +19112,7 @@
         <v>45012</v>
       </c>
       <c r="Q272" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="R272" t="s">
         <v>430</v>
@@ -19165,13 +19165,13 @@
         <v>45012</v>
       </c>
       <c r="Q273" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
       <c r="R273" t="s">
-        <v>1343</v>
+        <v>1332</v>
       </c>
       <c r="S273" t="s">
-        <v>1390</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="274" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -19218,13 +19218,13 @@
         <v>45012</v>
       </c>
       <c r="Q274" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="R274" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="S274" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="275" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -19271,13 +19271,13 @@
         <v>45012</v>
       </c>
       <c r="Q275" t="s">
-        <v>1388</v>
+        <v>1377</v>
       </c>
       <c r="R275" t="s">
-        <v>1389</v>
+        <v>1378</v>
       </c>
       <c r="S275" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="276" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -19324,13 +19324,13 @@
         <v>44978</v>
       </c>
       <c r="Q276" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="R276" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="S276" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="277" spans="2:19" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
changed "0" modification change in data set
</commit_message>
<xml_diff>
--- a/test_data/DataSetWithFullResults.xlsx
+++ b/test_data/DataSetWithFullResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobfehn/Documents/Uni/7. Semester/Thesis/Webservice/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0743317-6EF9-C948-AC0B-8C43E8B3FC4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F26A3D9-C87B-1E46-8DDC-74342D923FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{9DEADDE0-F9AA-D64D-B8E2-B7DD8B179BBE}"/>
   </bookViews>
@@ -4265,9 +4265,6 @@
     <t>C: 0 ; M: 1 + 9 ;</t>
   </si>
   <si>
-    <t>C: 0 ; M: 4 + 7 + 4 + 4 + 3 + 3 + 3 + 5 + 7 ;</t>
-  </si>
-  <si>
     <t>C: 0 ; M: 4 + 9 + 4 + 8 + 1 ;</t>
   </si>
   <si>
@@ -4488,6 +4485,9 @@
   </si>
   <si>
     <t>M13 with 0 mods (M9: 6-&gt;5)</t>
+  </si>
+  <si>
+    <t>C: 0 ; M: 4 + 7 + 4 + 3 + 1 + 3 + 3 + 3 + 5 + 7 ;</t>
   </si>
 </sst>
 </file>
@@ -4924,8 +4924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89784638-68A1-8249-8E72-BC8438B6227E}">
   <dimension ref="B1:T277"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O59" sqref="O59"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L277" sqref="L277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5371,7 +5371,7 @@
         <v>44978</v>
       </c>
       <c r="Q9" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="R9" t="s">
         <v>430</v>
@@ -5533,7 +5533,7 @@
         <v>44978</v>
       </c>
       <c r="Q12" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
       <c r="R12" t="s">
         <v>1256</v>
@@ -5786,16 +5786,16 @@
         <v>800</v>
       </c>
       <c r="O17" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="P17" s="4">
         <v>44978</v>
       </c>
       <c r="Q17" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="R17" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="S17" t="s">
         <v>1209</v>
@@ -6113,7 +6113,7 @@
         <v>1209</v>
       </c>
       <c r="R23" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
       <c r="S23" t="s">
         <v>1385</v>
@@ -6731,10 +6731,10 @@
         <v>44991</v>
       </c>
       <c r="Q35" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
       <c r="R35" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
       <c r="S35" t="s">
         <v>1388</v>
@@ -7361,10 +7361,10 @@
         <v>44992</v>
       </c>
       <c r="Q47" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="R47" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="S47" t="s">
         <v>1384</v>
@@ -7417,7 +7417,7 @@
         <v>1395</v>
       </c>
       <c r="R48" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="S48" t="s">
         <v>1396</v>
@@ -7900,7 +7900,7 @@
         <v>1225</v>
       </c>
       <c r="R57" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
       <c r="S57" t="s">
         <v>1273</v>
@@ -7947,13 +7947,13 @@
         <v>838</v>
       </c>
       <c r="O58" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
       <c r="P58" s="4">
         <v>44992</v>
       </c>
       <c r="Q58" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="R58" t="s">
         <v>1324</v>
@@ -7962,7 +7962,7 @@
         <v>1399</v>
       </c>
       <c r="T58" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="59" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -8165,22 +8165,22 @@
         <v>842</v>
       </c>
       <c r="O62" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="P62" s="4">
         <v>44992</v>
       </c>
       <c r="Q62" t="s">
-        <v>1402</v>
+        <v>1476</v>
       </c>
       <c r="R62" t="s">
         <v>1325</v>
       </c>
       <c r="S62" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="T62" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="63" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -8233,7 +8233,7 @@
         <v>1326</v>
       </c>
       <c r="S63" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="T63" t="s">
         <v>1315</v>
@@ -8280,13 +8280,13 @@
         <v>844</v>
       </c>
       <c r="O64" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="P64" s="4">
         <v>44992</v>
       </c>
       <c r="Q64" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="R64" t="s">
         <v>1215</v>
@@ -8548,13 +8548,13 @@
         <v>44992</v>
       </c>
       <c r="Q69" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="R69" t="s">
         <v>1217</v>
       </c>
       <c r="S69" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="70" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -8607,7 +8607,7 @@
         <v>1239</v>
       </c>
       <c r="S70" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="71" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -8710,7 +8710,7 @@
         <v>1328</v>
       </c>
       <c r="S72" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="73" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -8969,7 +8969,7 @@
         <v>1329</v>
       </c>
       <c r="S77" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="78" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -9022,7 +9022,7 @@
         <v>1330</v>
       </c>
       <c r="S78" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="79" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -9128,7 +9128,7 @@
         <v>1331</v>
       </c>
       <c r="S80" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="81" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -9381,10 +9381,10 @@
         <v>1240</v>
       </c>
       <c r="R85" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="S85" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="86" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -9490,7 +9490,7 @@
         <v>1209</v>
       </c>
       <c r="S87" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="88" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -9646,7 +9646,7 @@
         <v>1332</v>
       </c>
       <c r="S90" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="91" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -10111,10 +10111,10 @@
         <v>1210</v>
       </c>
       <c r="S99" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="T99" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="100" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -10476,7 +10476,7 @@
         <v>1210</v>
       </c>
       <c r="S106" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="107" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -10632,7 +10632,7 @@
         <v>1210</v>
       </c>
       <c r="S109" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="110" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -11044,7 +11044,7 @@
         <v>45012</v>
       </c>
       <c r="Q117" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="R117" t="s">
         <v>1268</v>
@@ -11106,7 +11106,7 @@
         <v>1386</v>
       </c>
       <c r="T118" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="119" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -11159,7 +11159,7 @@
         <v>1341</v>
       </c>
       <c r="S119" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="120" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -11206,13 +11206,13 @@
         <v>45012</v>
       </c>
       <c r="Q120" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="R120" t="s">
         <v>1343</v>
       </c>
       <c r="S120" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="121" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -11309,7 +11309,7 @@
         <v>45012</v>
       </c>
       <c r="Q122" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="R122" t="s">
         <v>430</v>
@@ -11318,7 +11318,7 @@
         <v>430</v>
       </c>
       <c r="T122" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="123" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -11362,7 +11362,7 @@
         <v>45012</v>
       </c>
       <c r="Q123" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="R123" t="s">
         <v>430</v>
@@ -11371,7 +11371,7 @@
         <v>430</v>
       </c>
       <c r="T123" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="124" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -11677,13 +11677,13 @@
         <v>45012</v>
       </c>
       <c r="Q129" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="R129" t="s">
         <v>1273</v>
       </c>
       <c r="S129" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="130" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -11736,7 +11736,7 @@
         <v>1215</v>
       </c>
       <c r="S130" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="131" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -11995,7 +11995,7 @@
         <v>1209</v>
       </c>
       <c r="S135" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="136" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -12257,7 +12257,7 @@
         <v>1215</v>
       </c>
       <c r="S140" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="141" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -12304,13 +12304,13 @@
         <v>45034</v>
       </c>
       <c r="Q141" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="R141" t="s">
         <v>1346</v>
       </c>
       <c r="S141" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="T141" t="s">
         <v>1315</v>
@@ -12357,7 +12357,7 @@
         <v>45034</v>
       </c>
       <c r="Q142" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="R142" t="s">
         <v>430</v>
@@ -12510,7 +12510,7 @@
         <v>45034</v>
       </c>
       <c r="Q145" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="R145" t="s">
         <v>430</v>
@@ -12937,13 +12937,13 @@
         <v>45034</v>
       </c>
       <c r="Q153" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="R153" t="s">
         <v>1349</v>
       </c>
       <c r="S153" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="154" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -13090,13 +13090,13 @@
         <v>45034</v>
       </c>
       <c r="Q156" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="R156" t="s">
         <v>1273</v>
       </c>
       <c r="S156" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="157" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -13199,7 +13199,7 @@
         <v>1350</v>
       </c>
       <c r="S158" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="159" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -13399,13 +13399,13 @@
         <v>45034</v>
       </c>
       <c r="Q162" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="R162" t="s">
         <v>1255</v>
       </c>
       <c r="S162" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="163" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -13770,7 +13770,7 @@
         <v>1215</v>
       </c>
       <c r="S169" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="170" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -14020,13 +14020,13 @@
         <v>951</v>
       </c>
       <c r="O174" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
       <c r="P174" s="4">
         <v>45034</v>
       </c>
       <c r="Q174" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="R174" t="s">
         <v>430</v>
@@ -14035,7 +14035,7 @@
         <v>430</v>
       </c>
       <c r="T174" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="175" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -14091,7 +14091,7 @@
         <v>430</v>
       </c>
       <c r="T175" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="176" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -14147,7 +14147,7 @@
         <v>1273</v>
       </c>
       <c r="S176" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="177" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -15003,7 +15003,7 @@
         <v>45034</v>
       </c>
       <c r="Q193" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="R193" t="s">
         <v>430</v>
@@ -15271,7 +15271,7 @@
         <v>1273</v>
       </c>
       <c r="S198" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="199" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -15786,7 +15786,7 @@
         <v>1358</v>
       </c>
       <c r="S208" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="T208" t="s">
         <v>1315</v>
@@ -15842,7 +15842,7 @@
         <v>1359</v>
       </c>
       <c r="S209" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="210" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -16157,7 +16157,7 @@
         <v>1363</v>
       </c>
       <c r="S215" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="216" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -16572,7 +16572,7 @@
         <v>1365</v>
       </c>
       <c r="S223" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="224" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -16675,7 +16675,7 @@
         <v>1215</v>
       </c>
       <c r="S225" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="226" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -16928,7 +16928,7 @@
         <v>1336</v>
       </c>
       <c r="S230" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="231" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -17090,7 +17090,7 @@
         <v>1291</v>
       </c>
       <c r="S233" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="234" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -17405,7 +17405,7 @@
         <v>1273</v>
       </c>
       <c r="S239" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="240" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -17555,13 +17555,13 @@
         <v>45012</v>
       </c>
       <c r="Q242" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
       <c r="R242" t="s">
         <v>1256</v>
       </c>
       <c r="S242" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="243" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -17767,7 +17767,7 @@
         <v>1209</v>
       </c>
       <c r="S246" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="247" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -17820,7 +17820,7 @@
         <v>1209</v>
       </c>
       <c r="S247" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="248" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -17873,7 +17873,7 @@
         <v>1336</v>
       </c>
       <c r="S248" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="249" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -17926,7 +17926,7 @@
         <v>1373</v>
       </c>
       <c r="S249" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="250" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -18344,7 +18344,7 @@
         <v>1341</v>
       </c>
       <c r="S257" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="258" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -18503,7 +18503,7 @@
         <v>1215</v>
       </c>
       <c r="S260" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="261" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -18865,7 +18865,7 @@
         <v>1247</v>
       </c>
       <c r="S267" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="268" spans="2:19" ht="18" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
some corrections of documentation
</commit_message>
<xml_diff>
--- a/test_data/DataSetWithFullResults.xlsx
+++ b/test_data/DataSetWithFullResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobfehn/Documents/Uni/7. Semester/Thesis/Webservice/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB36E56D-48FE-4E4F-A733-B637D5CB901D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0050419D-BC58-BC4B-8EF9-AD35284B951C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{9DEADDE0-F9AA-D64D-B8E2-B7DD8B179BBE}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3086" uniqueCount="1483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3086" uniqueCount="1482">
   <si>
     <t>Date First</t>
   </si>
@@ -3906,9 +3906,6 @@
     <t>C: 2 + 4 ; M: 3 + 1 + 1 + 3 + 1 ;</t>
   </si>
   <si>
-    <t>C: 2 + 1 ; M: 51 + 11 + 5 + 6 + 21 + 28 + 1 ;</t>
-  </si>
-  <si>
     <t>C: 9 ; M: 1 + 1 + 1 + 2 + 36 ;</t>
   </si>
   <si>
@@ -4095,9 +4092,6 @@
     <t>C: 0 ; M: 25 + 1 ;</t>
   </si>
   <si>
-    <t>C: 0 ; M: 0 ; (?)</t>
-  </si>
-  <si>
     <t>C: 0 ; M: 12 ;</t>
   </si>
   <si>
@@ -4365,9 +4359,6 @@
     <t>C: 1 ; M: 4 ;</t>
   </si>
   <si>
-    <t>C: 2 + 1 ; M: 51 + 9 + 5 + 5 + 21 ;</t>
-  </si>
-  <si>
     <t>C: 13 ; M: 1 + 1 + 1 + 2 ;</t>
   </si>
   <si>
@@ -4510,6 +4501,12 @@
   </si>
   <si>
     <t>Number of consolidated Versions</t>
+  </si>
+  <si>
+    <t>C: 2 + 1 + 1 ; M: 51 + 11 + 5 + 6 + 21 + 28 + 1 ;</t>
+  </si>
+  <si>
+    <t>C: 2 + 1 + 1 ; M: 51 + 9 + 5 + 5 + 21 ;</t>
   </si>
 </sst>
 </file>
@@ -10661,8 +10658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89784638-68A1-8249-8E72-BC8438B6227E}">
   <dimension ref="B1:T277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O161" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q174" sqref="Q174"/>
+    <sheetView tabSelected="1" topLeftCell="N193" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="T208" sqref="T208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10690,7 +10687,7 @@
   <sheetData>
     <row r="1" spans="2:19" x14ac:dyDescent="0.2">
       <c r="L1" t="s">
-        <v>1481</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="2" spans="2:19" x14ac:dyDescent="0.2">
@@ -10722,7 +10719,7 @@
         <v>586</v>
       </c>
       <c r="K2" t="s">
-        <v>1482</v>
+        <v>1479</v>
       </c>
       <c r="L2" t="s">
         <v>758</v>
@@ -10743,10 +10740,10 @@
         <v>1203</v>
       </c>
       <c r="R2" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="S2" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="3" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -10931,7 +10928,7 @@
         <v>2021</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="K6">
         <v>3</v>
@@ -10952,10 +10949,10 @@
         <v>44978</v>
       </c>
       <c r="Q6" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="R6" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="S6" t="s">
         <v>1271</v>
@@ -11005,13 +11002,13 @@
         <v>44978</v>
       </c>
       <c r="Q7" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="R7" t="s">
         <v>1213</v>
       </c>
       <c r="S7" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="8" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -11064,7 +11061,7 @@
         <v>1213</v>
       </c>
       <c r="S8" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="9" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -11108,7 +11105,7 @@
         <v>44978</v>
       </c>
       <c r="Q9" t="s">
-        <v>1443</v>
+        <v>1440</v>
       </c>
       <c r="R9" t="s">
         <v>430</v>
@@ -11161,10 +11158,10 @@
         <v>44978</v>
       </c>
       <c r="Q10" t="s">
+        <v>1309</v>
+      </c>
+      <c r="R10" t="s">
         <v>1310</v>
-      </c>
-      <c r="R10" t="s">
-        <v>1311</v>
       </c>
       <c r="S10" t="s">
         <v>1207</v>
@@ -11217,7 +11214,7 @@
         <v>44978</v>
       </c>
       <c r="Q11" t="s">
-        <v>1381</v>
+        <v>1379</v>
       </c>
       <c r="R11" t="s">
         <v>1208</v>
@@ -11270,13 +11267,13 @@
         <v>44978</v>
       </c>
       <c r="Q12" t="s">
-        <v>1467</v>
+        <v>1464</v>
       </c>
       <c r="R12" t="s">
         <v>1254</v>
       </c>
       <c r="S12" t="s">
-        <v>1380</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="13" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -11523,16 +11520,16 @@
         <v>799</v>
       </c>
       <c r="O17" t="s">
-        <v>1462</v>
+        <v>1459</v>
       </c>
       <c r="P17" s="4">
         <v>44978</v>
       </c>
       <c r="Q17" t="s">
-        <v>1451</v>
+        <v>1448</v>
       </c>
       <c r="R17" t="s">
-        <v>1451</v>
+        <v>1448</v>
       </c>
       <c r="S17" t="s">
         <v>1207</v>
@@ -11582,10 +11579,10 @@
         <v>44978</v>
       </c>
       <c r="Q18" t="s">
-        <v>1382</v>
+        <v>1380</v>
       </c>
       <c r="R18" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="S18" t="s">
         <v>1213</v>
@@ -11682,7 +11679,7 @@
         <v>44978</v>
       </c>
       <c r="Q20" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
       <c r="R20" t="s">
         <v>430</v>
@@ -11735,7 +11732,7 @@
         <v>44978</v>
       </c>
       <c r="Q21" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="R21" t="s">
         <v>1208</v>
@@ -11850,13 +11847,13 @@
         <v>1207</v>
       </c>
       <c r="R23" t="s">
-        <v>1463</v>
+        <v>1460</v>
       </c>
       <c r="S23" t="s">
-        <v>1383</v>
+        <v>1381</v>
       </c>
       <c r="T23" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="24" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -12012,7 +12009,7 @@
         <v>1207</v>
       </c>
       <c r="S26" t="s">
-        <v>1384</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="27" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -12056,7 +12053,7 @@
         <v>44991</v>
       </c>
       <c r="Q27" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
       <c r="R27" t="s">
         <v>430</v>
@@ -12262,10 +12259,10 @@
         <v>44991</v>
       </c>
       <c r="Q31" t="s">
-        <v>1385</v>
+        <v>1383</v>
       </c>
       <c r="R31" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="S31" t="s">
         <v>1215</v>
@@ -12415,10 +12412,10 @@
         <v>44991</v>
       </c>
       <c r="Q34" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="R34" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="S34" t="s">
         <v>1213</v>
@@ -12468,16 +12465,16 @@
         <v>44991</v>
       </c>
       <c r="Q35" t="s">
-        <v>1469</v>
+        <v>1466</v>
       </c>
       <c r="R35" t="s">
-        <v>1468</v>
+        <v>1465</v>
       </c>
       <c r="S35" t="s">
-        <v>1386</v>
+        <v>1384</v>
       </c>
       <c r="T35" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="36" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -12624,13 +12621,13 @@
         <v>44992</v>
       </c>
       <c r="Q38" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
       <c r="R38" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
       <c r="S38" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="39" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -12683,7 +12680,7 @@
         <v>1212</v>
       </c>
       <c r="S39" t="s">
-        <v>1388</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="40" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -12736,7 +12733,7 @@
         <v>1212</v>
       </c>
       <c r="S40" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="41" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -12783,13 +12780,13 @@
         <v>44992</v>
       </c>
       <c r="Q41" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="R41" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="S41" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="42" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -12842,7 +12839,7 @@
         <v>1212</v>
       </c>
       <c r="S42" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="43" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -12945,10 +12942,10 @@
         <v>1216</v>
       </c>
       <c r="R44" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="S44" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="45" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -13048,7 +13045,7 @@
         <v>1217</v>
       </c>
       <c r="R46" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="S46" t="s">
         <v>1207</v>
@@ -13098,13 +13095,13 @@
         <v>44992</v>
       </c>
       <c r="Q47" t="s">
-        <v>1452</v>
+        <v>1449</v>
       </c>
       <c r="R47" t="s">
-        <v>1464</v>
+        <v>1461</v>
       </c>
       <c r="S47" t="s">
-        <v>1382</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="48" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -13151,13 +13148,13 @@
         <v>44992</v>
       </c>
       <c r="Q48" t="s">
-        <v>1393</v>
+        <v>1391</v>
       </c>
       <c r="R48" t="s">
-        <v>1470</v>
+        <v>1467</v>
       </c>
       <c r="S48" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="49" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -13260,7 +13257,7 @@
         <v>1218</v>
       </c>
       <c r="R50" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="S50" t="s">
         <v>1207</v>
@@ -13313,13 +13310,13 @@
         <v>1219</v>
       </c>
       <c r="R51" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="S51" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="T51" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="52" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -13369,10 +13366,10 @@
         <v>1220</v>
       </c>
       <c r="R52" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="S52" t="s">
-        <v>1395</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="53" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -13422,7 +13419,7 @@
         <v>1221</v>
       </c>
       <c r="R53" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="S53" t="s">
         <v>1237</v>
@@ -13531,7 +13528,7 @@
         <v>1212</v>
       </c>
       <c r="S55" t="s">
-        <v>1396</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="56" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -13637,7 +13634,7 @@
         <v>1223</v>
       </c>
       <c r="R57" t="s">
-        <v>1465</v>
+        <v>1462</v>
       </c>
       <c r="S57" t="s">
         <v>1271</v>
@@ -13684,22 +13681,22 @@
         <v>837</v>
       </c>
       <c r="O58" t="s">
-        <v>1473</v>
+        <v>1470</v>
       </c>
       <c r="P58" s="4">
         <v>44992</v>
       </c>
       <c r="Q58" t="s">
-        <v>1471</v>
+        <v>1468</v>
       </c>
       <c r="R58" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="S58" t="s">
-        <v>1397</v>
+        <v>1395</v>
       </c>
       <c r="T58" t="s">
-        <v>1450</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="59" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -13752,7 +13749,7 @@
         <v>1207</v>
       </c>
       <c r="S59" t="s">
-        <v>1398</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="60" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -13802,10 +13799,10 @@
         <v>1225</v>
       </c>
       <c r="R60" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="S60" t="s">
-        <v>1399</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="61" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -13902,22 +13899,22 @@
         <v>841</v>
       </c>
       <c r="O62" t="s">
-        <v>1472</v>
+        <v>1469</v>
       </c>
       <c r="P62" s="4">
         <v>44992</v>
       </c>
       <c r="Q62" t="s">
-        <v>1474</v>
+        <v>1471</v>
       </c>
       <c r="R62" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="S62" t="s">
-        <v>1400</v>
+        <v>1398</v>
       </c>
       <c r="T62" t="s">
-        <v>1450</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="63" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -13964,16 +13961,16 @@
         <v>44992</v>
       </c>
       <c r="Q63" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="R63" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="S63" t="s">
-        <v>1401</v>
+        <v>1399</v>
       </c>
       <c r="T63" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="64" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -14017,13 +14014,13 @@
         <v>843</v>
       </c>
       <c r="O64" t="s">
-        <v>1466</v>
+        <v>1463</v>
       </c>
       <c r="P64" s="4">
         <v>44992</v>
       </c>
       <c r="Q64" t="s">
-        <v>1402</v>
+        <v>1400</v>
       </c>
       <c r="R64" t="s">
         <v>1213</v>
@@ -14032,7 +14029,7 @@
         <v>1264</v>
       </c>
       <c r="T64" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="65" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -14082,7 +14079,7 @@
         <v>1227</v>
       </c>
       <c r="R65" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="S65" t="s">
         <v>1213</v>
@@ -14285,13 +14282,13 @@
         <v>44992</v>
       </c>
       <c r="Q69" t="s">
-        <v>1403</v>
+        <v>1401</v>
       </c>
       <c r="R69" t="s">
         <v>1215</v>
       </c>
       <c r="S69" t="s">
-        <v>1404</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="70" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -14344,7 +14341,7 @@
         <v>1237</v>
       </c>
       <c r="S70" t="s">
-        <v>1405</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="71" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -14444,10 +14441,10 @@
         <v>1231</v>
       </c>
       <c r="R72" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="S72" t="s">
-        <v>1406</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="73" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -14653,7 +14650,7 @@
         <v>1271</v>
       </c>
       <c r="S76" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="77" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -14703,10 +14700,10 @@
         <v>1234</v>
       </c>
       <c r="R77" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="S77" t="s">
-        <v>1407</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="78" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -14756,10 +14753,10 @@
         <v>1235</v>
       </c>
       <c r="R78" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="S78" t="s">
-        <v>1408</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="79" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -14862,10 +14859,10 @@
         <v>1236</v>
       </c>
       <c r="R80" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="S80" t="s">
-        <v>1409</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="81" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -15118,10 +15115,10 @@
         <v>1238</v>
       </c>
       <c r="R85" t="s">
-        <v>1453</v>
+        <v>1450</v>
       </c>
       <c r="S85" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="86" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -15227,7 +15224,7 @@
         <v>1207</v>
       </c>
       <c r="S87" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="88" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -15294,7 +15291,7 @@
         <v>2016</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="G89">
         <v>2018</v>
@@ -15380,10 +15377,10 @@
         <v>1242</v>
       </c>
       <c r="R90" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="S90" t="s">
-        <v>1412</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="91" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -15433,7 +15430,7 @@
         <v>1243</v>
       </c>
       <c r="R91" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="S91" t="s">
         <v>1213</v>
@@ -15686,10 +15683,10 @@
         <v>1244</v>
       </c>
       <c r="R96" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="S96" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="97" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -15736,16 +15733,16 @@
         <v>45012</v>
       </c>
       <c r="Q97" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
       <c r="R97" t="s">
         <v>1204</v>
       </c>
       <c r="S97" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
       <c r="T97" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="98" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -15842,16 +15839,16 @@
         <v>45012</v>
       </c>
       <c r="Q99" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="R99" t="s">
         <v>1208</v>
       </c>
       <c r="S99" t="s">
-        <v>1413</v>
+        <v>1411</v>
       </c>
       <c r="T99" t="s">
-        <v>1450</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="100" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -15901,7 +15898,7 @@
         <v>1246</v>
       </c>
       <c r="R100" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="S100" t="s">
         <v>1209</v>
@@ -15954,10 +15951,10 @@
         <v>1247</v>
       </c>
       <c r="R101" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="S101" t="s">
-        <v>1384</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="102" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -16213,7 +16210,7 @@
         <v>1208</v>
       </c>
       <c r="S106" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="107" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -16369,7 +16366,7 @@
         <v>1208</v>
       </c>
       <c r="S109" t="s">
-        <v>1415</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="110" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -16569,7 +16566,7 @@
         <v>45012</v>
       </c>
       <c r="Q113" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="R113" t="s">
         <v>1207</v>
@@ -16781,7 +16778,7 @@
         <v>45012</v>
       </c>
       <c r="Q117" t="s">
-        <v>1416</v>
+        <v>1414</v>
       </c>
       <c r="R117" t="s">
         <v>1266</v>
@@ -16834,16 +16831,16 @@
         <v>45012</v>
       </c>
       <c r="Q118" t="s">
+        <v>1336</v>
+      </c>
+      <c r="R118" t="s">
         <v>1337</v>
       </c>
-      <c r="R118" t="s">
-        <v>1338</v>
-      </c>
       <c r="S118" t="s">
-        <v>1384</v>
+        <v>1382</v>
       </c>
       <c r="T118" t="s">
-        <v>1450</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="119" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -16890,13 +16887,13 @@
         <v>45012</v>
       </c>
       <c r="Q119" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="R119" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="S119" t="s">
-        <v>1417</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="120" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -16943,13 +16940,13 @@
         <v>45012</v>
       </c>
       <c r="Q120" t="s">
-        <v>1454</v>
+        <v>1451</v>
       </c>
       <c r="R120" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="S120" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="121" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -17046,7 +17043,7 @@
         <v>45012</v>
       </c>
       <c r="Q122" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
       <c r="R122" t="s">
         <v>430</v>
@@ -17055,7 +17052,7 @@
         <v>430</v>
       </c>
       <c r="T122" t="s">
-        <v>1450</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="123" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -17099,7 +17096,7 @@
         <v>45012</v>
       </c>
       <c r="Q123" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
       <c r="R123" t="s">
         <v>430</v>
@@ -17108,7 +17105,7 @@
         <v>430</v>
       </c>
       <c r="T123" t="s">
-        <v>1450</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="124" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -17261,7 +17258,7 @@
         <v>45012</v>
       </c>
       <c r="Q126" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="R126" t="s">
         <v>1213</v>
@@ -17311,7 +17308,7 @@
         <v>45012</v>
       </c>
       <c r="Q127" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
       <c r="R127" t="s">
         <v>430</v>
@@ -17361,7 +17358,7 @@
         <v>45012</v>
       </c>
       <c r="Q128" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="R128" t="s">
         <v>430</v>
@@ -17414,13 +17411,13 @@
         <v>45012</v>
       </c>
       <c r="Q129" t="s">
-        <v>1455</v>
+        <v>1452</v>
       </c>
       <c r="R129" t="s">
         <v>1271</v>
       </c>
       <c r="S129" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="130" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -17473,7 +17470,7 @@
         <v>1213</v>
       </c>
       <c r="S130" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="131" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -17732,7 +17729,7 @@
         <v>1207</v>
       </c>
       <c r="S135" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="136" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -17782,7 +17779,7 @@
         <v>1256</v>
       </c>
       <c r="R136" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="S136" t="s">
         <v>1207</v>
@@ -17994,7 +17991,7 @@
         <v>1213</v>
       </c>
       <c r="S140" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="141" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -18041,16 +18038,16 @@
         <v>45034</v>
       </c>
       <c r="Q141" t="s">
-        <v>1425</v>
+        <v>1423</v>
       </c>
       <c r="R141" t="s">
-        <v>1344</v>
+        <v>1204</v>
       </c>
       <c r="S141" t="s">
-        <v>1426</v>
+        <v>1424</v>
       </c>
       <c r="T141" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="142" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -18094,7 +18091,7 @@
         <v>45034</v>
       </c>
       <c r="Q142" t="s">
-        <v>1456</v>
+        <v>1453</v>
       </c>
       <c r="R142" t="s">
         <v>430</v>
@@ -18200,7 +18197,7 @@
         <v>1259</v>
       </c>
       <c r="R144" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="S144" t="s">
         <v>1207</v>
@@ -18247,7 +18244,7 @@
         <v>45034</v>
       </c>
       <c r="Q145" t="s">
-        <v>1457</v>
+        <v>1454</v>
       </c>
       <c r="R145" t="s">
         <v>430</v>
@@ -18300,16 +18297,16 @@
         <v>45034</v>
       </c>
       <c r="Q146" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="R146" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="S146" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="T146" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="147" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -18624,10 +18621,10 @@
         <v>1261</v>
       </c>
       <c r="R152" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="S152" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="153" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -18674,13 +18671,13 @@
         <v>45034</v>
       </c>
       <c r="Q153" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
       <c r="R153" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="S153" t="s">
-        <v>1428</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="154" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -18827,13 +18824,13 @@
         <v>45034</v>
       </c>
       <c r="Q156" t="s">
-        <v>1458</v>
+        <v>1455</v>
       </c>
       <c r="R156" t="s">
         <v>1271</v>
       </c>
       <c r="S156" t="s">
-        <v>1429</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="157" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -18933,10 +18930,10 @@
         <v>1262</v>
       </c>
       <c r="R158" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="S158" t="s">
-        <v>1430</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="159" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -19136,13 +19133,13 @@
         <v>45034</v>
       </c>
       <c r="Q162" t="s">
-        <v>1449</v>
+        <v>1446</v>
       </c>
       <c r="R162" t="s">
         <v>1253</v>
       </c>
       <c r="S162" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="163" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -19242,10 +19239,10 @@
         <v>1263</v>
       </c>
       <c r="R164" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="S164" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="165" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -19401,7 +19398,7 @@
         <v>1208</v>
       </c>
       <c r="S167" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="168" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -19507,7 +19504,7 @@
         <v>1213</v>
       </c>
       <c r="S169" t="s">
-        <v>1432</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="170" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -19604,10 +19601,10 @@
         <v>45034</v>
       </c>
       <c r="Q171" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="R171" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="S171" t="s">
         <v>1207</v>
@@ -19757,13 +19754,13 @@
         <v>950</v>
       </c>
       <c r="O174" t="s">
-        <v>1461</v>
+        <v>1458</v>
       </c>
       <c r="P174" s="4">
         <v>45034</v>
       </c>
       <c r="Q174" t="s">
-        <v>1451</v>
+        <v>1448</v>
       </c>
       <c r="R174" t="s">
         <v>430</v>
@@ -19772,7 +19769,7 @@
         <v>430</v>
       </c>
       <c r="T174" t="s">
-        <v>1450</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="175" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -19828,7 +19825,7 @@
         <v>430</v>
       </c>
       <c r="T175" t="s">
-        <v>1450</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="176" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -19884,7 +19881,7 @@
         <v>1271</v>
       </c>
       <c r="S176" t="s">
-        <v>1415</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="177" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -20034,7 +20031,7 @@
         <v>1270</v>
       </c>
       <c r="R179" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
       <c r="S179" t="s">
         <v>1254</v>
@@ -20590,7 +20587,7 @@
         <v>1272</v>
       </c>
       <c r="R190" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="S190" t="s">
         <v>1213</v>
@@ -20643,7 +20640,7 @@
         <v>1273</v>
       </c>
       <c r="R191" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="S191" t="s">
         <v>1207</v>
@@ -20740,7 +20737,7 @@
         <v>45034</v>
       </c>
       <c r="Q193" t="s">
-        <v>1460</v>
+        <v>1457</v>
       </c>
       <c r="R193" t="s">
         <v>430</v>
@@ -20846,7 +20843,7 @@
         <v>1246</v>
       </c>
       <c r="R195" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="S195" t="s">
         <v>1209</v>
@@ -20899,7 +20896,7 @@
         <v>1274</v>
       </c>
       <c r="R196" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
       <c r="S196" t="s">
         <v>1207</v>
@@ -20952,7 +20949,7 @@
         <v>1275</v>
       </c>
       <c r="R197" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="S197" t="s">
         <v>1214</v>
@@ -21008,7 +21005,7 @@
         <v>1271</v>
       </c>
       <c r="S198" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="199" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -21064,7 +21061,7 @@
         <v>1258</v>
       </c>
       <c r="T199" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="200" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -21164,10 +21161,10 @@
         <v>1277</v>
       </c>
       <c r="R201" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
       <c r="S201" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="202" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -21367,7 +21364,7 @@
         <v>1243</v>
       </c>
       <c r="R205" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="S205" t="s">
         <v>1213</v>
@@ -21517,16 +21514,16 @@
         <v>45034</v>
       </c>
       <c r="Q208" t="s">
-        <v>1281</v>
+        <v>1480</v>
       </c>
       <c r="R208" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="S208" t="s">
-        <v>1434</v>
+        <v>1481</v>
       </c>
       <c r="T208" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="209" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -21573,13 +21570,13 @@
         <v>45034</v>
       </c>
       <c r="Q209" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="R209" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="S209" t="s">
-        <v>1435</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="210" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -21676,13 +21673,13 @@
         <v>45034</v>
       </c>
       <c r="Q211" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="R211" t="s">
         <v>1213</v>
       </c>
       <c r="S211" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="212" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -21782,7 +21779,7 @@
         <v>45034</v>
       </c>
       <c r="Q213" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="R213" t="s">
         <v>1215</v>
@@ -21835,10 +21832,10 @@
         <v>45034</v>
       </c>
       <c r="Q214" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
       <c r="R214" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
       <c r="S214" t="s">
         <v>1207</v>
@@ -21888,13 +21885,13 @@
         <v>45012</v>
       </c>
       <c r="Q215" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
       <c r="R215" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
       <c r="S215" t="s">
-        <v>1436</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="216" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -21941,7 +21938,7 @@
         <v>45012</v>
       </c>
       <c r="Q216" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="R216" t="s">
         <v>1237</v>
@@ -21994,10 +21991,10 @@
         <v>45012</v>
       </c>
       <c r="Q217" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="R217" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
       <c r="S217" t="s">
         <v>1213</v>
@@ -22097,13 +22094,13 @@
         <v>45012</v>
       </c>
       <c r="Q219" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="R219" t="s">
         <v>1208</v>
       </c>
       <c r="S219" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="220" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -22303,13 +22300,13 @@
         <v>45012</v>
       </c>
       <c r="Q223" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="R223" t="s">
-        <v>1363</v>
+        <v>1361</v>
       </c>
       <c r="S223" t="s">
-        <v>1437</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="224" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -22412,7 +22409,7 @@
         <v>1213</v>
       </c>
       <c r="S225" t="s">
-        <v>1438</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="226" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -22456,7 +22453,7 @@
         <v>45012</v>
       </c>
       <c r="Q226" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="R226" t="s">
         <v>430</v>
@@ -22659,13 +22656,13 @@
         <v>45012</v>
       </c>
       <c r="Q230" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="R230" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="S230" t="s">
-        <v>1439</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="231" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -22712,10 +22709,10 @@
         <v>45012</v>
       </c>
       <c r="Q231" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
       <c r="R231" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
       <c r="S231" t="s">
         <v>1215</v>
@@ -22765,16 +22762,16 @@
         <v>45012</v>
       </c>
       <c r="Q232" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="R232" t="s">
+        <v>1311</v>
+      </c>
+      <c r="S232" t="s">
+        <v>1333</v>
+      </c>
+      <c r="T232" t="s">
         <v>1312</v>
-      </c>
-      <c r="S232" t="s">
-        <v>1334</v>
-      </c>
-      <c r="T232" t="s">
-        <v>1313</v>
       </c>
     </row>
     <row r="233" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -22821,13 +22818,13 @@
         <v>45012</v>
       </c>
       <c r="Q233" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="R233" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="S233" t="s">
-        <v>1440</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="234" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -22874,10 +22871,10 @@
         <v>45012</v>
       </c>
       <c r="Q234" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="R234" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
       <c r="S234" t="s">
         <v>1214</v>
@@ -22927,10 +22924,10 @@
         <v>45012</v>
       </c>
       <c r="Q235" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="R235" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="S235" t="s">
         <v>1207</v>
@@ -22980,13 +22977,13 @@
         <v>45012</v>
       </c>
       <c r="Q236" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
       <c r="R236" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
       <c r="S236" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="237" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -23086,7 +23083,7 @@
         <v>1275</v>
       </c>
       <c r="R238" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="S238" t="s">
         <v>1214</v>
@@ -23142,7 +23139,7 @@
         <v>1271</v>
       </c>
       <c r="S239" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="240" spans="2:20" ht="18" x14ac:dyDescent="0.2">
@@ -23292,13 +23289,13 @@
         <v>45012</v>
       </c>
       <c r="Q242" t="s">
-        <v>1459</v>
+        <v>1456</v>
       </c>
       <c r="R242" t="s">
         <v>1254</v>
       </c>
       <c r="S242" t="s">
-        <v>1441</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="243" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -23395,13 +23392,13 @@
         <v>45012</v>
       </c>
       <c r="Q244" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="R244" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
       <c r="S244" t="s">
-        <v>1395</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="245" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -23504,7 +23501,7 @@
         <v>1207</v>
       </c>
       <c r="S246" t="s">
-        <v>1442</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="247" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -23551,13 +23548,13 @@
         <v>45012</v>
       </c>
       <c r="Q247" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="R247" t="s">
         <v>1207</v>
       </c>
       <c r="S247" t="s">
-        <v>1443</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="248" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -23607,10 +23604,10 @@
         <v>1277</v>
       </c>
       <c r="R248" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="S248" t="s">
-        <v>1444</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="249" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -23657,13 +23654,13 @@
         <v>45012</v>
       </c>
       <c r="Q249" t="s">
-        <v>1370</v>
+        <v>1368</v>
       </c>
       <c r="R249" t="s">
-        <v>1371</v>
+        <v>1369</v>
       </c>
       <c r="S249" t="s">
-        <v>1445</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="250" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -23813,13 +23810,13 @@
         <v>45012</v>
       </c>
       <c r="Q252" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="R252" t="s">
         <v>1204</v>
       </c>
       <c r="S252" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="253" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -24022,13 +24019,13 @@
         <v>45012</v>
       </c>
       <c r="Q256" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="R256" t="s">
         <v>1271</v>
       </c>
       <c r="S256" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="257" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -24075,13 +24072,13 @@
         <v>45012</v>
       </c>
       <c r="Q257" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="R257" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="S257" t="s">
-        <v>1446</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="258" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -24181,10 +24178,10 @@
         <v>45012</v>
       </c>
       <c r="Q259" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="R259" t="s">
-        <v>1372</v>
+        <v>1370</v>
       </c>
       <c r="S259" t="s">
         <v>1207</v>
@@ -24234,13 +24231,13 @@
         <v>45012</v>
       </c>
       <c r="Q260" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="R260" t="s">
         <v>1213</v>
       </c>
       <c r="S260" t="s">
-        <v>1447</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="261" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -24387,7 +24384,7 @@
         <v>45012</v>
       </c>
       <c r="Q263" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="R263" t="s">
         <v>1213</v>
@@ -24493,10 +24490,10 @@
         <v>45012</v>
       </c>
       <c r="Q265" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="R265" t="s">
-        <v>1373</v>
+        <v>1371</v>
       </c>
       <c r="S265" t="s">
         <v>1207</v>
@@ -24596,13 +24593,13 @@
         <v>45012</v>
       </c>
       <c r="Q267" t="s">
-        <v>1374</v>
+        <v>1372</v>
       </c>
       <c r="R267" t="s">
         <v>1245</v>
       </c>
       <c r="S267" t="s">
-        <v>1448</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="268" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -24799,7 +24796,7 @@
         <v>45012</v>
       </c>
       <c r="Q271" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="R271" t="s">
         <v>1207</v>
@@ -24902,13 +24899,13 @@
         <v>45012</v>
       </c>
       <c r="Q273" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="R273" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="S273" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="274" spans="2:19" ht="18" x14ac:dyDescent="0.2">
@@ -25008,10 +25005,10 @@
         <v>45012</v>
       </c>
       <c r="Q275" t="s">
-        <v>1375</v>
+        <v>1373</v>
       </c>
       <c r="R275" t="s">
-        <v>1376</v>
+        <v>1374</v>
       </c>
       <c r="S275" t="s">
         <v>1260</v>
@@ -26088,7 +26085,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D1" t="s">
-        <v>1479</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -26096,13 +26093,13 @@
         <v>758</v>
       </c>
       <c r="B2" t="s">
+        <v>1472</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1474</v>
+      </c>
+      <c r="D2" t="s">
         <v>1475</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1477</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1478</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -26395,7 +26392,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>1476</v>
+        <v>1473</v>
       </c>
       <c r="B24" s="5">
         <v>274</v>
@@ -26411,7 +26408,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
-        <v>1480</v>
+        <v>1477</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
problem with data set
</commit_message>
<xml_diff>
--- a/test_data/DataSetWithFullResults.xlsx
+++ b/test_data/DataSetWithFullResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobfehn/Documents/Uni/7. Semester/Thesis/Webservice/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041300C1-600C-AC41-A467-3CD5AD27E3E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101426B3-27A5-A347-8944-3D3B47DA15F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{9DEADDE0-F9AA-D64D-B8E2-B7DD8B179BBE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{9DEADDE0-F9AA-D64D-B8E2-B7DD8B179BBE}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3104" uniqueCount="1495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3103" uniqueCount="1495">
   <si>
     <t>Date First</t>
   </si>
@@ -10696,8 +10696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89784638-68A1-8249-8E72-BC8438B6227E}">
   <dimension ref="B1:T277"/>
   <sheetViews>
-    <sheetView topLeftCell="G16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11517,7 +11517,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="17" spans="2:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:19" ht="18" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>17</v>
       </c>
@@ -11573,7 +11573,7 @@
         <v>1207</v>
       </c>
     </row>
-    <row r="18" spans="2:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:19" ht="18" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>18</v>
       </c>
@@ -11626,7 +11626,7 @@
         <v>1213</v>
       </c>
     </row>
-    <row r="19" spans="2:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:19" ht="18" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>19</v>
       </c>
@@ -11676,7 +11676,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="20" spans="2:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:19" ht="18" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>20</v>
       </c>
@@ -11726,7 +11726,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="21" spans="2:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:19" ht="18" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>21</v>
       </c>
@@ -11779,7 +11779,7 @@
         <v>1207</v>
       </c>
     </row>
-    <row r="22" spans="2:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:19" ht="18" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>22</v>
       </c>
@@ -11835,7 +11835,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="23" spans="2:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:19" ht="18" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>23</v>
       </c>
@@ -11890,11 +11890,8 @@
       <c r="S23" t="s">
         <v>1381</v>
       </c>
-      <c r="T23" t="s">
-        <v>1312</v>
-      </c>
-    </row>
-    <row r="24" spans="2:20" ht="18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="2:19" ht="18" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>24</v>
       </c>
@@ -11944,7 +11941,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="25" spans="2:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:19" ht="18" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>25</v>
       </c>
@@ -11997,7 +11994,7 @@
         <v>1213</v>
       </c>
     </row>
-    <row r="26" spans="2:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:19" ht="18" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>26</v>
       </c>
@@ -12050,7 +12047,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="27" spans="2:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:19" ht="18" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>27</v>
       </c>
@@ -12100,7 +12097,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="28" spans="2:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:19" ht="18" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>28</v>
       </c>
@@ -12150,7 +12147,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="29" spans="2:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:19" ht="18" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>29</v>
       </c>
@@ -12200,7 +12197,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="30" spans="2:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:19" ht="18" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>30</v>
       </c>
@@ -12253,7 +12250,7 @@
         <v>1213</v>
       </c>
     </row>
-    <row r="31" spans="2:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:19" ht="18" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>31</v>
       </c>
@@ -12306,7 +12303,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="32" spans="2:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:19" ht="18" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>32</v>
       </c>
@@ -26110,7 +26107,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0ADA798-A6CF-F247-800F-5E07B8C41610}">
   <dimension ref="A2:W32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
problem with no print
</commit_message>
<xml_diff>
--- a/test_data/DataSetWithFullResults.xlsx
+++ b/test_data/DataSetWithFullResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobfehn/Documents/Uni/7. Semester/Thesis/Webservice/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101426B3-27A5-A347-8944-3D3B47DA15F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D52A6661-3F9E-6645-A96E-5BD7E40BB8C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{9DEADDE0-F9AA-D64D-B8E2-B7DD8B179BBE}"/>
   </bookViews>
@@ -10696,8 +10696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89784638-68A1-8249-8E72-BC8438B6227E}">
   <dimension ref="B1:T277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26108,7 +26108,7 @@
   <dimension ref="A2:W32"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added problematic qualitative testing
</commit_message>
<xml_diff>
--- a/test_data/DataSetWithFullResults.xlsx
+++ b/test_data/DataSetWithFullResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobfehn/Documents/Uni/7. Semester/Thesis/Webservice/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A45A40-8239-104B-8C90-902C0D4876C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E555182-3CC2-454B-8BE0-269661EBB6A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{9DEADDE0-F9AA-D64D-B8E2-B7DD8B179BBE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" xr2:uid="{9DEADDE0-F9AA-D64D-B8E2-B7DD8B179BBE}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId3"/>
+    <pivotCache cacheId="5" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -10360,7 +10360,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00D48549-437D-FB46-A6B8-82A7A224A508}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00D48549-437D-FB46-A6B8-82A7A224A508}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A2:B24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="18">
     <pivotField compact="0" outline="0" showAll="0"/>
@@ -10822,8 +10822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89784638-68A1-8249-8E72-BC8438B6227E}">
   <dimension ref="B1:T277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P89" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="T97" sqref="T97"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>